<commit_message>
delete security zone service
</commit_message>
<xml_diff>
--- a/flask-backend/Rack Info-201703.xlsx
+++ b/flask-backend/Rack Info-201703.xlsx
@@ -5,17 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="201703" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$66</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_24821951_458D_4863_863B_0C0B4A6350AE_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$66</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_F725D54E_BA8A_4561_B030_7A250C390FCD_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$66</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_F930B092_4476_4D77_A695_E370DC8CEE30_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$66</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$66</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_24821951_458D_4863_863B_0C0B4A6350AE_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_F725D54E_BA8A_4561_B030_7A250C390FCD_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_F930B092_4476_4D77_A695_E370DC8CEE30_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1059">
   <si>
     <t xml:space="preserve">R00 - R11003</t>
   </si>
@@ -3376,9 +3376,6 @@
     <t xml:space="preserve">S14057</t>
   </si>
   <si>
-    <t xml:space="preserve">ADMIN</t>
-  </si>
-  <si>
     <t xml:space="preserve">Administrator</t>
   </si>
   <si>
@@ -3413,9 +3410,6 @@
   </si>
   <si>
     <t xml:space="preserve">BIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMS(T2)</t>
   </si>
   <si>
     <t xml:space="preserve">CMS</t>
@@ -3432,7 +3426,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-_-;_-@_-"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3589,12 +3583,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -6399,7 +6387,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6688,22 +6676,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="3" borderId="4" xfId="671" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="23" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6721,10 +6705,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="25" borderId="4" xfId="670" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="20" borderId="4" xfId="672" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7459,13 +7439,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65"/>
+  <dimension ref="1:64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A46" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.2834008097166"/>
@@ -62147,353 +62127,353 @@
       <c r="AMJ50" s="0"/>
     </row>
     <row r="51" s="8" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C51" s="72" t="s">
+      <c r="C51" s="46" t="s">
         <v>1045</v>
       </c>
-      <c r="F51" s="73"/>
+      <c r="F51" s="72"/>
       <c r="H51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="K51" s="72"/>
+      <c r="M51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="P51" s="72"/>
+      <c r="R51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="U51" s="72"/>
+      <c r="W51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Z51" s="72"/>
+      <c r="AB51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AE51" s="72"/>
+      <c r="AG51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AJ51" s="72"/>
+      <c r="AL51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AO51" s="72"/>
+      <c r="AQ51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AT51" s="72"/>
+      <c r="AV51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="AY51" s="72"/>
+      <c r="BA51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BD51" s="72"/>
+      <c r="BF51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BI51" s="72"/>
+      <c r="BK51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BN51" s="72"/>
+      <c r="BP51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BS51" s="72"/>
+      <c r="BU51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BX51" s="72"/>
+      <c r="BZ51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="CC51" s="72"/>
+      <c r="CE51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="CH51" s="72"/>
+      <c r="CJ51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="CM51" s="72"/>
+      <c r="CO51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="CR51" s="72"/>
+      <c r="CT51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="CW51" s="72"/>
+      <c r="CY51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="DB51" s="72"/>
+      <c r="DD51" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="DG51" s="72"/>
+      <c r="DI51" s="46" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="52" s="73" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="K51" s="73"/>
-      <c r="M51" s="46" t="s">
+      <c r="F52" s="74"/>
+      <c r="H52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="P51" s="73"/>
-      <c r="R51" s="46" t="s">
+      <c r="K52" s="74"/>
+      <c r="M52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="U51" s="73"/>
-      <c r="W51" s="46" t="s">
+      <c r="P52" s="74"/>
+      <c r="R52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="Z51" s="73"/>
-      <c r="AB51" s="46" t="s">
+      <c r="T52" s="8"/>
+      <c r="U52" s="74"/>
+      <c r="W52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="AE51" s="73"/>
-      <c r="AG51" s="46" t="s">
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="74"/>
+      <c r="AB52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="AJ51" s="73"/>
-      <c r="AL51" s="46" t="s">
+      <c r="AE52" s="74"/>
+      <c r="AG52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="AO51" s="73"/>
-      <c r="AQ51" s="46" t="s">
+      <c r="AJ52" s="74"/>
+      <c r="AL52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="AT51" s="73"/>
-      <c r="AV51" s="46" t="s">
+      <c r="AN52" s="8"/>
+      <c r="AO52" s="74"/>
+      <c r="AQ52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="AY51" s="73"/>
-      <c r="BA51" s="46" t="s">
+      <c r="AT52" s="74"/>
+      <c r="AV52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="BD51" s="73"/>
-      <c r="BF51" s="46" t="s">
+      <c r="AY52" s="74"/>
+      <c r="BA52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="BI51" s="73"/>
-      <c r="BK51" s="46" t="s">
+      <c r="BD52" s="74"/>
+      <c r="BF52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="BN51" s="73"/>
-      <c r="BP51" s="46" t="s">
+      <c r="BI52" s="74"/>
+      <c r="BK52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="BS51" s="73"/>
-      <c r="BU51" s="46" t="s">
+      <c r="BN52" s="74"/>
+      <c r="BP52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="BX51" s="73"/>
-      <c r="BZ51" s="46" t="s">
+      <c r="BS52" s="74"/>
+      <c r="BU52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="CC51" s="73"/>
-      <c r="CE51" s="46" t="s">
+      <c r="BX52" s="74"/>
+      <c r="BZ52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="CH51" s="73"/>
-      <c r="CJ51" s="46" t="s">
+      <c r="CC52" s="74"/>
+      <c r="CE52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="CM51" s="73"/>
-      <c r="CO51" s="46" t="s">
+      <c r="CH52" s="74"/>
+      <c r="CJ52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="CR51" s="73"/>
-      <c r="CT51" s="46" t="s">
+      <c r="CM52" s="74"/>
+      <c r="CO52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="CW51" s="73"/>
-      <c r="CY51" s="46" t="s">
+      <c r="CR52" s="74"/>
+      <c r="CT52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="DB51" s="73"/>
-      <c r="DD51" s="46" t="s">
+      <c r="CW52" s="74"/>
+      <c r="CY52" s="32" t="s">
         <v>1046</v>
       </c>
-      <c r="DG51" s="73"/>
-      <c r="DI51" s="46" t="s">
+      <c r="DB52" s="74"/>
+      <c r="DD52" s="32" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="52" s="74" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="F52" s="75"/>
-      <c r="H52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="K52" s="75"/>
-      <c r="M52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="P52" s="75"/>
-      <c r="R52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="T52" s="8"/>
-      <c r="U52" s="75"/>
-      <c r="W52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="Y52" s="8"/>
-      <c r="Z52" s="75"/>
-      <c r="AB52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AE52" s="75"/>
-      <c r="AG52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AJ52" s="75"/>
-      <c r="AL52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AN52" s="8"/>
-      <c r="AO52" s="75"/>
-      <c r="AQ52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AT52" s="75"/>
-      <c r="AV52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="AY52" s="75"/>
-      <c r="BA52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="BD52" s="75"/>
-      <c r="BF52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="BI52" s="75"/>
-      <c r="BK52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="BN52" s="75"/>
-      <c r="BP52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="BS52" s="75"/>
-      <c r="BU52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="BX52" s="75"/>
-      <c r="BZ52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="CC52" s="75"/>
-      <c r="CE52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="CH52" s="75"/>
-      <c r="CJ52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="CM52" s="75"/>
-      <c r="CO52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="CR52" s="75"/>
-      <c r="CT52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="CW52" s="75"/>
-      <c r="CY52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="DB52" s="75"/>
-      <c r="DD52" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="DG52" s="75"/>
+      <c r="DG52" s="74"/>
       <c r="DI52" s="32" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
-      <c r="C53" s="76" t="s">
-        <v>1048</v>
+      <c r="C53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
       <c r="G53" s="0"/>
-      <c r="H53" s="76" t="s">
-        <v>1048</v>
+      <c r="H53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="I53" s="0"/>
       <c r="J53" s="0"/>
       <c r="K53" s="0"/>
       <c r="L53" s="0"/>
-      <c r="M53" s="76" t="s">
-        <v>1048</v>
+      <c r="M53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="N53" s="0"/>
       <c r="O53" s="0"/>
       <c r="P53" s="0"/>
       <c r="Q53" s="0"/>
-      <c r="R53" s="76" t="s">
-        <v>1048</v>
+      <c r="R53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="S53" s="0"/>
       <c r="T53" s="3"/>
       <c r="U53" s="0"/>
       <c r="V53" s="0"/>
-      <c r="W53" s="76" t="s">
-        <v>1048</v>
+      <c r="W53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="X53" s="0"/>
       <c r="Y53" s="3"/>
       <c r="Z53" s="0"/>
       <c r="AA53" s="0"/>
-      <c r="AB53" s="76" t="s">
-        <v>1048</v>
+      <c r="AB53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="AC53" s="0"/>
       <c r="AD53" s="1"/>
       <c r="AE53" s="0"/>
       <c r="AF53" s="0"/>
-      <c r="AG53" s="76" t="s">
-        <v>1048</v>
+      <c r="AG53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="AH53" s="0"/>
       <c r="AI53" s="1"/>
       <c r="AJ53" s="0"/>
       <c r="AK53" s="0"/>
-      <c r="AL53" s="76" t="s">
-        <v>1048</v>
+      <c r="AL53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="AM53" s="0"/>
       <c r="AN53" s="3"/>
       <c r="AO53" s="0"/>
       <c r="AP53" s="0"/>
-      <c r="AQ53" s="76" t="s">
-        <v>1048</v>
+      <c r="AQ53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="AR53" s="0"/>
       <c r="AS53" s="0"/>
       <c r="AT53" s="0"/>
       <c r="AU53" s="0"/>
-      <c r="AV53" s="76" t="s">
-        <v>1048</v>
+      <c r="AV53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="AW53" s="0"/>
       <c r="AX53" s="1"/>
       <c r="AY53" s="0"/>
       <c r="AZ53" s="0"/>
-      <c r="BA53" s="76" t="s">
-        <v>1048</v>
+      <c r="BA53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="BB53" s="0"/>
       <c r="BC53" s="0"/>
       <c r="BD53" s="0"/>
       <c r="BE53" s="0"/>
-      <c r="BF53" s="76" t="s">
-        <v>1048</v>
+      <c r="BF53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="BG53" s="0"/>
       <c r="BH53" s="0"/>
       <c r="BI53" s="0"/>
       <c r="BJ53" s="0"/>
-      <c r="BK53" s="76" t="s">
-        <v>1048</v>
+      <c r="BK53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="BL53" s="0"/>
       <c r="BM53" s="0"/>
       <c r="BN53" s="0"/>
       <c r="BO53" s="0"/>
-      <c r="BP53" s="76" t="s">
-        <v>1048</v>
+      <c r="BP53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="BQ53" s="0"/>
       <c r="BR53" s="0"/>
       <c r="BS53" s="0"/>
       <c r="BT53" s="0"/>
-      <c r="BU53" s="76" t="s">
-        <v>1048</v>
+      <c r="BU53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="BV53" s="0"/>
       <c r="BW53" s="0"/>
       <c r="BX53" s="0"/>
       <c r="BY53" s="0"/>
-      <c r="BZ53" s="76" t="s">
-        <v>1048</v>
+      <c r="BZ53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CA53" s="0"/>
       <c r="CB53" s="0"/>
       <c r="CC53" s="0"/>
       <c r="CD53" s="0"/>
-      <c r="CE53" s="76" t="s">
-        <v>1048</v>
+      <c r="CE53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CF53" s="0"/>
       <c r="CG53" s="0"/>
       <c r="CH53" s="2"/>
       <c r="CI53" s="0"/>
-      <c r="CJ53" s="76" t="s">
-        <v>1048</v>
+      <c r="CJ53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CK53" s="0"/>
       <c r="CL53" s="0"/>
       <c r="CM53" s="2"/>
       <c r="CN53" s="0"/>
-      <c r="CO53" s="76" t="s">
-        <v>1048</v>
+      <c r="CO53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CP53" s="0"/>
       <c r="CQ53" s="0"/>
       <c r="CR53" s="2"/>
       <c r="CS53" s="0"/>
-      <c r="CT53" s="76" t="s">
-        <v>1048</v>
+      <c r="CT53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CU53" s="0"/>
       <c r="CV53" s="0"/>
       <c r="CW53" s="2"/>
       <c r="CX53" s="0"/>
-      <c r="CY53" s="76" t="s">
-        <v>1048</v>
+      <c r="CY53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="CZ53" s="0"/>
       <c r="DA53" s="0"/>
       <c r="DB53" s="2"/>
       <c r="DC53" s="0"/>
-      <c r="DD53" s="76" t="s">
-        <v>1048</v>
+      <c r="DD53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="DE53" s="0"/>
       <c r="DF53" s="0"/>
       <c r="DG53" s="2"/>
       <c r="DH53" s="0"/>
-      <c r="DI53" s="76" t="s">
-        <v>1048</v>
+      <c r="DI53" s="75" t="s">
+        <v>1047</v>
       </c>
       <c r="DJ53" s="0"/>
       <c r="DK53" s="0"/>
@@ -63411,161 +63391,161 @@
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
       <c r="C54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D54" s="0"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
       <c r="G54" s="0"/>
       <c r="H54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="I54" s="0"/>
       <c r="J54" s="0"/>
       <c r="K54" s="0"/>
       <c r="L54" s="0"/>
       <c r="M54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="N54" s="0"/>
       <c r="O54" s="0"/>
       <c r="P54" s="0"/>
       <c r="Q54" s="0"/>
       <c r="R54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="S54" s="0"/>
       <c r="T54" s="3"/>
       <c r="U54" s="0"/>
       <c r="V54" s="0"/>
       <c r="W54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="X54" s="0"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="0"/>
       <c r="AA54" s="0"/>
       <c r="AB54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AC54" s="0"/>
       <c r="AD54" s="1"/>
       <c r="AE54" s="0"/>
       <c r="AF54" s="0"/>
       <c r="AG54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AH54" s="0"/>
       <c r="AI54" s="1"/>
       <c r="AJ54" s="0"/>
       <c r="AK54" s="0"/>
       <c r="AL54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AM54" s="0"/>
       <c r="AN54" s="3"/>
       <c r="AO54" s="0"/>
       <c r="AP54" s="0"/>
       <c r="AQ54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AR54" s="0"/>
       <c r="AS54" s="0"/>
       <c r="AT54" s="0"/>
       <c r="AU54" s="0"/>
       <c r="AV54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="AW54" s="0"/>
       <c r="AX54" s="1"/>
       <c r="AY54" s="0"/>
       <c r="AZ54" s="0"/>
       <c r="BA54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BB54" s="0"/>
       <c r="BC54" s="0"/>
       <c r="BD54" s="0"/>
       <c r="BE54" s="0"/>
       <c r="BF54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BG54" s="0"/>
       <c r="BH54" s="0"/>
       <c r="BI54" s="0"/>
       <c r="BJ54" s="0"/>
       <c r="BK54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BL54" s="0"/>
       <c r="BM54" s="0"/>
       <c r="BN54" s="0"/>
       <c r="BO54" s="0"/>
       <c r="BP54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BQ54" s="0"/>
       <c r="BR54" s="0"/>
       <c r="BS54" s="0"/>
       <c r="BT54" s="0"/>
       <c r="BU54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="BV54" s="0"/>
       <c r="BW54" s="0"/>
       <c r="BX54" s="0"/>
       <c r="BY54" s="0"/>
       <c r="BZ54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CA54" s="0"/>
       <c r="CB54" s="0"/>
       <c r="CC54" s="0"/>
       <c r="CD54" s="0"/>
       <c r="CE54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CF54" s="0"/>
       <c r="CG54" s="0"/>
       <c r="CH54" s="2"/>
       <c r="CI54" s="0"/>
       <c r="CJ54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CK54" s="0"/>
       <c r="CL54" s="0"/>
       <c r="CM54" s="2"/>
       <c r="CN54" s="0"/>
       <c r="CO54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CP54" s="0"/>
       <c r="CQ54" s="0"/>
       <c r="CR54" s="2"/>
       <c r="CS54" s="0"/>
       <c r="CT54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CU54" s="0"/>
       <c r="CV54" s="0"/>
       <c r="CW54" s="2"/>
       <c r="CX54" s="0"/>
       <c r="CY54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="CZ54" s="0"/>
       <c r="DA54" s="0"/>
       <c r="DB54" s="2"/>
       <c r="DC54" s="0"/>
       <c r="DD54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="DE54" s="0"/>
       <c r="DF54" s="0"/>
       <c r="DG54" s="2"/>
       <c r="DH54" s="0"/>
       <c r="DI54" s="44" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="DJ54" s="0"/>
       <c r="DK54" s="0"/>
@@ -64479,258 +64459,258 @@
       <c r="AMI54" s="0"/>
       <c r="AMJ54" s="0"/>
     </row>
-    <row r="55" s="74" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="F55" s="75"/>
-      <c r="H55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="K55" s="75"/>
-      <c r="M55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="P55" s="75"/>
-      <c r="R55" s="77" t="s">
-        <v>1050</v>
+    <row r="55" s="73" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F55" s="74"/>
+      <c r="H55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="K55" s="74"/>
+      <c r="M55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P55" s="74"/>
+      <c r="R55" s="76" t="s">
+        <v>1049</v>
       </c>
       <c r="T55" s="8"/>
-      <c r="U55" s="75"/>
-      <c r="W55" s="77" t="s">
-        <v>1050</v>
+      <c r="U55" s="74"/>
+      <c r="W55" s="76" t="s">
+        <v>1049</v>
       </c>
       <c r="Y55" s="8"/>
-      <c r="Z55" s="75"/>
-      <c r="AB55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="AE55" s="75"/>
-      <c r="AG55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="AJ55" s="75"/>
-      <c r="AL55" s="77" t="s">
-        <v>1050</v>
+      <c r="Z55" s="74"/>
+      <c r="AB55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AE55" s="74"/>
+      <c r="AG55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AJ55" s="74"/>
+      <c r="AL55" s="76" t="s">
+        <v>1049</v>
       </c>
       <c r="AN55" s="8"/>
-      <c r="AO55" s="75"/>
-      <c r="AQ55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="AT55" s="75"/>
-      <c r="AV55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="AY55" s="75"/>
-      <c r="BA55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="BD55" s="75"/>
-      <c r="BF55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="BI55" s="75"/>
-      <c r="BK55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="BN55" s="75"/>
-      <c r="BP55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="BS55" s="75"/>
-      <c r="BU55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="BX55" s="75"/>
-      <c r="BZ55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="CC55" s="75"/>
-      <c r="CE55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="CH55" s="75"/>
-      <c r="CJ55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="CM55" s="75"/>
-      <c r="CO55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="CR55" s="75"/>
-      <c r="CT55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="CW55" s="75"/>
-      <c r="CY55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="DB55" s="75"/>
-      <c r="DD55" s="77" t="s">
-        <v>1050</v>
-      </c>
-      <c r="DG55" s="75"/>
-      <c r="DI55" s="77" t="s">
-        <v>1050</v>
+      <c r="AO55" s="74"/>
+      <c r="AQ55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AT55" s="74"/>
+      <c r="AV55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AY55" s="74"/>
+      <c r="BA55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BD55" s="74"/>
+      <c r="BF55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BI55" s="74"/>
+      <c r="BK55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BN55" s="74"/>
+      <c r="BP55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BS55" s="74"/>
+      <c r="BU55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BX55" s="74"/>
+      <c r="BZ55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="CC55" s="74"/>
+      <c r="CE55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="CH55" s="74"/>
+      <c r="CJ55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="CM55" s="74"/>
+      <c r="CO55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="CR55" s="74"/>
+      <c r="CT55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="CW55" s="74"/>
+      <c r="CY55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="DB55" s="74"/>
+      <c r="DD55" s="76" t="s">
+        <v>1049</v>
+      </c>
+      <c r="DG55" s="74"/>
+      <c r="DI55" s="76" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
       <c r="B56" s="0"/>
       <c r="C56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D56" s="0"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
       <c r="G56" s="0"/>
       <c r="H56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="I56" s="0"/>
       <c r="J56" s="0"/>
       <c r="K56" s="0"/>
       <c r="L56" s="0"/>
       <c r="M56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="N56" s="0"/>
       <c r="O56" s="0"/>
       <c r="P56" s="0"/>
       <c r="Q56" s="0"/>
       <c r="R56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="S56" s="0"/>
       <c r="T56" s="3"/>
       <c r="U56" s="0"/>
       <c r="V56" s="0"/>
       <c r="W56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="X56" s="0"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="0"/>
       <c r="AA56" s="0"/>
       <c r="AB56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AC56" s="0"/>
       <c r="AE56" s="0"/>
       <c r="AF56" s="0"/>
       <c r="AG56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AH56" s="0"/>
       <c r="AJ56" s="0"/>
       <c r="AK56" s="0"/>
       <c r="AL56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AM56" s="0"/>
       <c r="AN56" s="3"/>
       <c r="AO56" s="0"/>
       <c r="AP56" s="0"/>
       <c r="AQ56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AR56" s="0"/>
       <c r="AS56" s="0"/>
       <c r="AT56" s="0"/>
       <c r="AU56" s="0"/>
       <c r="AV56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="AW56" s="0"/>
       <c r="AY56" s="0"/>
       <c r="AZ56" s="0"/>
       <c r="BA56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BB56" s="0"/>
       <c r="BC56" s="0"/>
       <c r="BD56" s="0"/>
       <c r="BE56" s="0"/>
       <c r="BF56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BG56" s="0"/>
       <c r="BH56" s="0"/>
       <c r="BI56" s="0"/>
       <c r="BJ56" s="0"/>
       <c r="BK56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BL56" s="0"/>
       <c r="BM56" s="0"/>
       <c r="BN56" s="0"/>
       <c r="BO56" s="0"/>
       <c r="BP56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BQ56" s="0"/>
       <c r="BR56" s="0"/>
       <c r="BS56" s="0"/>
       <c r="BT56" s="0"/>
       <c r="BU56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="BV56" s="0"/>
       <c r="BW56" s="0"/>
       <c r="BX56" s="0"/>
       <c r="BY56" s="0"/>
       <c r="BZ56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CA56" s="0"/>
       <c r="CB56" s="0"/>
       <c r="CC56" s="0"/>
       <c r="CD56" s="0"/>
       <c r="CE56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CF56" s="0"/>
       <c r="CG56" s="0"/>
       <c r="CH56" s="2"/>
       <c r="CI56" s="0"/>
       <c r="CJ56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CK56" s="0"/>
       <c r="CL56" s="0"/>
       <c r="CM56" s="2"/>
       <c r="CN56" s="0"/>
       <c r="CO56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CP56" s="0"/>
       <c r="CQ56" s="0"/>
       <c r="CR56" s="2"/>
       <c r="CS56" s="0"/>
       <c r="CT56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CU56" s="0"/>
       <c r="CV56" s="0"/>
       <c r="CW56" s="2"/>
       <c r="CX56" s="0"/>
       <c r="CY56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="CZ56" s="0"/>
       <c r="DA56" s="0"/>
       <c r="DB56" s="2"/>
       <c r="DC56" s="0"/>
       <c r="DD56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="DE56" s="0"/>
       <c r="DF56" s="0"/>
       <c r="DG56" s="2"/>
       <c r="DH56" s="0"/>
       <c r="DI56" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="DJ56" s="0"/>
       <c r="DK56" s="0"/>
@@ -64739,158 +64719,158 @@
       <c r="A57" s="0"/>
       <c r="B57" s="0"/>
       <c r="C57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D57" s="0"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
       <c r="G57" s="0"/>
       <c r="H57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="I57" s="0"/>
       <c r="J57" s="0"/>
       <c r="K57" s="0"/>
       <c r="L57" s="0"/>
       <c r="M57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="N57" s="0"/>
       <c r="O57" s="0"/>
       <c r="P57" s="0"/>
       <c r="Q57" s="0"/>
       <c r="R57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="S57" s="0"/>
       <c r="T57" s="3"/>
       <c r="U57" s="0"/>
       <c r="V57" s="0"/>
       <c r="W57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="X57" s="0"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="0"/>
       <c r="AA57" s="0"/>
       <c r="AB57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AC57" s="0"/>
       <c r="AE57" s="0"/>
       <c r="AF57" s="0"/>
       <c r="AG57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AH57" s="0"/>
       <c r="AJ57" s="0"/>
       <c r="AK57" s="0"/>
       <c r="AL57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AM57" s="0"/>
       <c r="AN57" s="3"/>
       <c r="AO57" s="0"/>
       <c r="AP57" s="0"/>
       <c r="AQ57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AR57" s="0"/>
       <c r="AS57" s="0"/>
       <c r="AT57" s="0"/>
       <c r="AU57" s="0"/>
       <c r="AV57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="AW57" s="0"/>
       <c r="AY57" s="0"/>
       <c r="AZ57" s="0"/>
       <c r="BA57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BB57" s="0"/>
       <c r="BC57" s="0"/>
       <c r="BD57" s="0"/>
       <c r="BE57" s="0"/>
       <c r="BF57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BG57" s="0"/>
       <c r="BH57" s="0"/>
       <c r="BI57" s="0"/>
       <c r="BJ57" s="0"/>
       <c r="BK57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BL57" s="0"/>
       <c r="BM57" s="0"/>
       <c r="BN57" s="0"/>
       <c r="BO57" s="0"/>
       <c r="BP57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BQ57" s="0"/>
       <c r="BR57" s="0"/>
       <c r="BS57" s="0"/>
       <c r="BT57" s="0"/>
       <c r="BU57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="BV57" s="0"/>
       <c r="BW57" s="0"/>
       <c r="BX57" s="0"/>
       <c r="BY57" s="0"/>
       <c r="BZ57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CA57" s="0"/>
       <c r="CB57" s="0"/>
       <c r="CC57" s="0"/>
       <c r="CD57" s="0"/>
       <c r="CE57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CF57" s="0"/>
       <c r="CG57" s="0"/>
       <c r="CH57" s="2"/>
       <c r="CI57" s="0"/>
       <c r="CJ57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CK57" s="0"/>
       <c r="CL57" s="0"/>
       <c r="CM57" s="2"/>
       <c r="CN57" s="0"/>
       <c r="CO57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CP57" s="0"/>
       <c r="CQ57" s="0"/>
       <c r="CR57" s="2"/>
       <c r="CS57" s="0"/>
       <c r="CT57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CU57" s="0"/>
       <c r="CV57" s="0"/>
       <c r="CW57" s="2"/>
       <c r="CX57" s="0"/>
       <c r="CY57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="CZ57" s="0"/>
       <c r="DA57" s="0"/>
       <c r="DB57" s="2"/>
       <c r="DC57" s="0"/>
       <c r="DD57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="DE57" s="0"/>
       <c r="DF57" s="0"/>
       <c r="DG57" s="2"/>
       <c r="DH57" s="0"/>
       <c r="DI57" s="45" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="DJ57" s="0"/>
       <c r="DK57" s="0"/>
@@ -64898,159 +64878,159 @@
     <row r="58" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0"/>
       <c r="B58" s="0"/>
-      <c r="C58" s="78" t="s">
-        <v>1053</v>
+      <c r="C58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
       <c r="G58" s="0"/>
-      <c r="H58" s="78" t="s">
-        <v>1053</v>
+      <c r="H58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="I58" s="0"/>
       <c r="J58" s="0"/>
       <c r="K58" s="0"/>
       <c r="L58" s="0"/>
-      <c r="M58" s="78" t="s">
-        <v>1053</v>
+      <c r="M58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="N58" s="0"/>
       <c r="O58" s="0"/>
       <c r="P58" s="0"/>
       <c r="Q58" s="0"/>
-      <c r="R58" s="78" t="s">
-        <v>1053</v>
+      <c r="R58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="S58" s="0"/>
       <c r="T58" s="3"/>
       <c r="U58" s="0"/>
       <c r="V58" s="0"/>
-      <c r="W58" s="78" t="s">
-        <v>1053</v>
+      <c r="W58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="X58" s="0"/>
       <c r="Y58" s="3"/>
       <c r="Z58" s="0"/>
       <c r="AA58" s="0"/>
-      <c r="AB58" s="78" t="s">
-        <v>1053</v>
+      <c r="AB58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="AC58" s="0"/>
       <c r="AE58" s="0"/>
       <c r="AF58" s="0"/>
-      <c r="AG58" s="78" t="s">
-        <v>1053</v>
+      <c r="AG58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="AH58" s="0"/>
       <c r="AJ58" s="0"/>
       <c r="AK58" s="0"/>
-      <c r="AL58" s="78" t="s">
-        <v>1053</v>
+      <c r="AL58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="AM58" s="0"/>
       <c r="AN58" s="3"/>
       <c r="AO58" s="0"/>
       <c r="AP58" s="0"/>
-      <c r="AQ58" s="78" t="s">
-        <v>1053</v>
+      <c r="AQ58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="AR58" s="0"/>
       <c r="AS58" s="0"/>
       <c r="AT58" s="0"/>
       <c r="AU58" s="0"/>
-      <c r="AV58" s="78" t="s">
-        <v>1053</v>
+      <c r="AV58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="AW58" s="0"/>
       <c r="AY58" s="0"/>
       <c r="AZ58" s="0"/>
-      <c r="BA58" s="78" t="s">
-        <v>1053</v>
+      <c r="BA58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="BB58" s="0"/>
       <c r="BC58" s="0"/>
       <c r="BD58" s="0"/>
       <c r="BE58" s="0"/>
-      <c r="BF58" s="78" t="s">
-        <v>1053</v>
+      <c r="BF58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="BG58" s="0"/>
       <c r="BH58" s="0"/>
       <c r="BI58" s="0"/>
       <c r="BJ58" s="0"/>
-      <c r="BK58" s="78" t="s">
-        <v>1053</v>
+      <c r="BK58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="BL58" s="0"/>
       <c r="BM58" s="0"/>
       <c r="BN58" s="0"/>
       <c r="BO58" s="0"/>
-      <c r="BP58" s="78" t="s">
-        <v>1053</v>
+      <c r="BP58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="BQ58" s="0"/>
       <c r="BR58" s="0"/>
       <c r="BS58" s="0"/>
       <c r="BT58" s="0"/>
-      <c r="BU58" s="78" t="s">
-        <v>1053</v>
+      <c r="BU58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="BV58" s="0"/>
       <c r="BW58" s="0"/>
       <c r="BX58" s="0"/>
       <c r="BY58" s="0"/>
-      <c r="BZ58" s="78" t="s">
-        <v>1053</v>
+      <c r="BZ58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CA58" s="0"/>
       <c r="CB58" s="0"/>
       <c r="CC58" s="0"/>
       <c r="CD58" s="0"/>
-      <c r="CE58" s="78" t="s">
-        <v>1053</v>
+      <c r="CE58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CF58" s="0"/>
       <c r="CG58" s="0"/>
       <c r="CH58" s="2"/>
       <c r="CI58" s="0"/>
-      <c r="CJ58" s="78" t="s">
-        <v>1053</v>
+      <c r="CJ58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CK58" s="0"/>
       <c r="CL58" s="0"/>
       <c r="CM58" s="2"/>
       <c r="CN58" s="0"/>
-      <c r="CO58" s="78" t="s">
-        <v>1053</v>
+      <c r="CO58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CP58" s="0"/>
       <c r="CQ58" s="0"/>
       <c r="CR58" s="2"/>
       <c r="CS58" s="0"/>
-      <c r="CT58" s="78" t="s">
-        <v>1053</v>
+      <c r="CT58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CU58" s="0"/>
       <c r="CV58" s="0"/>
       <c r="CW58" s="2"/>
       <c r="CX58" s="0"/>
-      <c r="CY58" s="78" t="s">
-        <v>1053</v>
+      <c r="CY58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="CZ58" s="0"/>
       <c r="DA58" s="0"/>
       <c r="DB58" s="2"/>
       <c r="DC58" s="0"/>
-      <c r="DD58" s="78" t="s">
-        <v>1053</v>
+      <c r="DD58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="DE58" s="0"/>
       <c r="DF58" s="0"/>
       <c r="DG58" s="2"/>
       <c r="DH58" s="0"/>
-      <c r="DI58" s="78" t="s">
-        <v>1053</v>
+      <c r="DI58" s="77" t="s">
+        <v>1052</v>
       </c>
       <c r="DJ58" s="0"/>
       <c r="DK58" s="0"/>
@@ -65059,158 +65039,158 @@
       <c r="A59" s="0"/>
       <c r="B59" s="0"/>
       <c r="C59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D59" s="0"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
       <c r="G59" s="0"/>
       <c r="H59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="I59" s="0"/>
       <c r="J59" s="0"/>
       <c r="K59" s="0"/>
       <c r="L59" s="0"/>
       <c r="M59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="N59" s="0"/>
       <c r="O59" s="0"/>
       <c r="P59" s="0"/>
       <c r="Q59" s="0"/>
       <c r="R59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="S59" s="0"/>
       <c r="T59" s="3"/>
       <c r="U59" s="0"/>
       <c r="V59" s="0"/>
       <c r="W59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="X59" s="0"/>
       <c r="Y59" s="3"/>
       <c r="Z59" s="0"/>
       <c r="AA59" s="0"/>
       <c r="AB59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AC59" s="0"/>
       <c r="AE59" s="0"/>
       <c r="AF59" s="0"/>
       <c r="AG59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AH59" s="0"/>
       <c r="AJ59" s="0"/>
       <c r="AK59" s="0"/>
       <c r="AL59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AM59" s="0"/>
       <c r="AN59" s="3"/>
       <c r="AO59" s="0"/>
       <c r="AP59" s="0"/>
       <c r="AQ59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AR59" s="0"/>
       <c r="AS59" s="0"/>
       <c r="AT59" s="0"/>
       <c r="AU59" s="0"/>
       <c r="AV59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="AW59" s="0"/>
       <c r="AY59" s="0"/>
       <c r="AZ59" s="0"/>
       <c r="BA59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BB59" s="0"/>
       <c r="BC59" s="0"/>
       <c r="BD59" s="0"/>
       <c r="BE59" s="0"/>
       <c r="BF59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BG59" s="0"/>
       <c r="BH59" s="0"/>
       <c r="BI59" s="0"/>
       <c r="BJ59" s="0"/>
       <c r="BK59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BL59" s="0"/>
       <c r="BM59" s="0"/>
       <c r="BN59" s="0"/>
       <c r="BO59" s="0"/>
       <c r="BP59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BQ59" s="0"/>
       <c r="BR59" s="0"/>
       <c r="BS59" s="0"/>
       <c r="BT59" s="0"/>
       <c r="BU59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="BV59" s="0"/>
       <c r="BW59" s="0"/>
       <c r="BX59" s="0"/>
       <c r="BY59" s="0"/>
       <c r="BZ59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CA59" s="0"/>
       <c r="CB59" s="0"/>
       <c r="CC59" s="0"/>
       <c r="CD59" s="0"/>
       <c r="CE59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CF59" s="0"/>
       <c r="CG59" s="0"/>
       <c r="CH59" s="2"/>
       <c r="CI59" s="0"/>
       <c r="CJ59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CK59" s="0"/>
       <c r="CL59" s="0"/>
       <c r="CM59" s="2"/>
       <c r="CN59" s="0"/>
       <c r="CO59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CP59" s="0"/>
       <c r="CQ59" s="0"/>
       <c r="CR59" s="2"/>
       <c r="CS59" s="0"/>
       <c r="CT59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CU59" s="0"/>
       <c r="CV59" s="0"/>
       <c r="CW59" s="2"/>
       <c r="CX59" s="0"/>
       <c r="CY59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="CZ59" s="0"/>
       <c r="DA59" s="0"/>
       <c r="DB59" s="2"/>
       <c r="DC59" s="0"/>
       <c r="DD59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="DE59" s="0"/>
       <c r="DF59" s="0"/>
       <c r="DG59" s="2"/>
       <c r="DH59" s="0"/>
       <c r="DI59" s="43" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="DJ59" s="0"/>
       <c r="DK59" s="0"/>
@@ -65218,159 +65198,159 @@
     <row r="60" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0"/>
       <c r="B60" s="0"/>
-      <c r="C60" s="79" t="s">
-        <v>1055</v>
+      <c r="C60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="D60" s="0"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
       <c r="G60" s="0"/>
-      <c r="H60" s="79" t="s">
-        <v>1055</v>
+      <c r="H60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="I60" s="0"/>
       <c r="J60" s="0"/>
       <c r="K60" s="0"/>
       <c r="L60" s="0"/>
-      <c r="M60" s="79" t="s">
-        <v>1055</v>
+      <c r="M60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="N60" s="0"/>
       <c r="O60" s="0"/>
       <c r="P60" s="0"/>
       <c r="Q60" s="0"/>
-      <c r="R60" s="79" t="s">
-        <v>1055</v>
+      <c r="R60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="S60" s="0"/>
       <c r="T60" s="3"/>
       <c r="U60" s="0"/>
       <c r="V60" s="0"/>
-      <c r="W60" s="79" t="s">
-        <v>1055</v>
+      <c r="W60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="X60" s="0"/>
       <c r="Y60" s="3"/>
       <c r="Z60" s="0"/>
       <c r="AA60" s="0"/>
-      <c r="AB60" s="79" t="s">
-        <v>1055</v>
+      <c r="AB60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="AC60" s="0"/>
       <c r="AE60" s="0"/>
       <c r="AF60" s="0"/>
-      <c r="AG60" s="79" t="s">
-        <v>1055</v>
+      <c r="AG60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="AH60" s="0"/>
       <c r="AJ60" s="0"/>
       <c r="AK60" s="0"/>
-      <c r="AL60" s="79" t="s">
-        <v>1055</v>
+      <c r="AL60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="AM60" s="0"/>
       <c r="AN60" s="3"/>
       <c r="AO60" s="0"/>
       <c r="AP60" s="0"/>
-      <c r="AQ60" s="79" t="s">
-        <v>1055</v>
+      <c r="AQ60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="AR60" s="0"/>
       <c r="AS60" s="0"/>
       <c r="AT60" s="0"/>
       <c r="AU60" s="0"/>
-      <c r="AV60" s="79" t="s">
-        <v>1055</v>
+      <c r="AV60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="AW60" s="0"/>
       <c r="AY60" s="0"/>
       <c r="AZ60" s="0"/>
-      <c r="BA60" s="79" t="s">
-        <v>1055</v>
+      <c r="BA60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="BB60" s="0"/>
       <c r="BC60" s="0"/>
       <c r="BD60" s="0"/>
       <c r="BE60" s="0"/>
-      <c r="BF60" s="79" t="s">
-        <v>1055</v>
+      <c r="BF60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="BG60" s="0"/>
       <c r="BH60" s="0"/>
       <c r="BI60" s="0"/>
       <c r="BJ60" s="0"/>
-      <c r="BK60" s="79" t="s">
-        <v>1055</v>
+      <c r="BK60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="BL60" s="0"/>
       <c r="BM60" s="0"/>
       <c r="BN60" s="0"/>
       <c r="BO60" s="0"/>
-      <c r="BP60" s="79" t="s">
-        <v>1055</v>
+      <c r="BP60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="BQ60" s="0"/>
       <c r="BR60" s="0"/>
       <c r="BS60" s="0"/>
       <c r="BT60" s="0"/>
-      <c r="BU60" s="79" t="s">
-        <v>1055</v>
+      <c r="BU60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="BV60" s="0"/>
       <c r="BW60" s="0"/>
       <c r="BX60" s="0"/>
       <c r="BY60" s="0"/>
-      <c r="BZ60" s="79" t="s">
-        <v>1055</v>
+      <c r="BZ60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CA60" s="0"/>
       <c r="CB60" s="0"/>
       <c r="CC60" s="0"/>
       <c r="CD60" s="0"/>
-      <c r="CE60" s="79" t="s">
-        <v>1055</v>
+      <c r="CE60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CF60" s="0"/>
       <c r="CG60" s="0"/>
       <c r="CH60" s="2"/>
       <c r="CI60" s="0"/>
-      <c r="CJ60" s="79" t="s">
-        <v>1055</v>
+      <c r="CJ60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CK60" s="0"/>
       <c r="CL60" s="0"/>
       <c r="CM60" s="2"/>
       <c r="CN60" s="0"/>
-      <c r="CO60" s="79" t="s">
-        <v>1055</v>
+      <c r="CO60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CP60" s="0"/>
       <c r="CQ60" s="0"/>
       <c r="CR60" s="2"/>
       <c r="CS60" s="0"/>
-      <c r="CT60" s="79" t="s">
-        <v>1055</v>
+      <c r="CT60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CU60" s="0"/>
       <c r="CV60" s="0"/>
       <c r="CW60" s="2"/>
       <c r="CX60" s="0"/>
-      <c r="CY60" s="79" t="s">
-        <v>1055</v>
+      <c r="CY60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="CZ60" s="0"/>
       <c r="DA60" s="0"/>
       <c r="DB60" s="2"/>
       <c r="DC60" s="0"/>
-      <c r="DD60" s="79" t="s">
-        <v>1055</v>
+      <c r="DD60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="DE60" s="0"/>
       <c r="DF60" s="0"/>
       <c r="DG60" s="2"/>
       <c r="DH60" s="0"/>
-      <c r="DI60" s="79" t="s">
-        <v>1055</v>
+      <c r="DI60" s="78" t="s">
+        <v>1054</v>
       </c>
       <c r="DJ60" s="0"/>
       <c r="DK60" s="0"/>
@@ -65378,159 +65358,159 @@
     <row r="61" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0"/>
       <c r="B61" s="0"/>
-      <c r="C61" s="80" t="s">
-        <v>1056</v>
+      <c r="C61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
       <c r="G61" s="0"/>
-      <c r="H61" s="80" t="s">
-        <v>1056</v>
+      <c r="H61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="I61" s="0"/>
       <c r="J61" s="0"/>
       <c r="K61" s="0"/>
       <c r="L61" s="0"/>
-      <c r="M61" s="80" t="s">
-        <v>1056</v>
+      <c r="M61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="N61" s="0"/>
       <c r="O61" s="0"/>
       <c r="P61" s="0"/>
       <c r="Q61" s="0"/>
-      <c r="R61" s="80" t="s">
-        <v>1056</v>
+      <c r="R61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="S61" s="0"/>
       <c r="T61" s="3"/>
       <c r="U61" s="0"/>
       <c r="V61" s="0"/>
-      <c r="W61" s="80" t="s">
-        <v>1056</v>
+      <c r="W61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="X61" s="0"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="0"/>
       <c r="AA61" s="0"/>
-      <c r="AB61" s="80" t="s">
-        <v>1056</v>
+      <c r="AB61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="AC61" s="0"/>
       <c r="AE61" s="0"/>
       <c r="AF61" s="0"/>
-      <c r="AG61" s="80" t="s">
-        <v>1056</v>
+      <c r="AG61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="AH61" s="0"/>
       <c r="AJ61" s="0"/>
       <c r="AK61" s="0"/>
-      <c r="AL61" s="80" t="s">
-        <v>1056</v>
+      <c r="AL61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="AM61" s="0"/>
       <c r="AN61" s="3"/>
       <c r="AO61" s="0"/>
       <c r="AP61" s="0"/>
-      <c r="AQ61" s="80" t="s">
-        <v>1056</v>
+      <c r="AQ61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="AR61" s="0"/>
       <c r="AS61" s="0"/>
       <c r="AT61" s="0"/>
       <c r="AU61" s="0"/>
-      <c r="AV61" s="80" t="s">
-        <v>1056</v>
+      <c r="AV61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="AW61" s="0"/>
       <c r="AY61" s="0"/>
       <c r="AZ61" s="0"/>
-      <c r="BA61" s="80" t="s">
-        <v>1056</v>
+      <c r="BA61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="BB61" s="0"/>
       <c r="BC61" s="0"/>
       <c r="BD61" s="0"/>
       <c r="BE61" s="0"/>
-      <c r="BF61" s="80" t="s">
-        <v>1056</v>
+      <c r="BF61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="BG61" s="0"/>
       <c r="BH61" s="0"/>
       <c r="BI61" s="0"/>
       <c r="BJ61" s="0"/>
-      <c r="BK61" s="80" t="s">
-        <v>1056</v>
+      <c r="BK61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="BL61" s="0"/>
       <c r="BM61" s="0"/>
       <c r="BN61" s="0"/>
       <c r="BO61" s="0"/>
-      <c r="BP61" s="80" t="s">
-        <v>1056</v>
+      <c r="BP61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="BQ61" s="0"/>
       <c r="BR61" s="0"/>
       <c r="BS61" s="0"/>
       <c r="BT61" s="0"/>
-      <c r="BU61" s="80" t="s">
-        <v>1056</v>
+      <c r="BU61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="BV61" s="0"/>
       <c r="BW61" s="0"/>
       <c r="BX61" s="0"/>
       <c r="BY61" s="0"/>
-      <c r="BZ61" s="80" t="s">
-        <v>1056</v>
+      <c r="BZ61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CA61" s="0"/>
       <c r="CB61" s="0"/>
       <c r="CC61" s="0"/>
       <c r="CD61" s="0"/>
-      <c r="CE61" s="80" t="s">
-        <v>1056</v>
+      <c r="CE61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CF61" s="0"/>
       <c r="CG61" s="0"/>
       <c r="CH61" s="2"/>
       <c r="CI61" s="0"/>
-      <c r="CJ61" s="80" t="s">
-        <v>1056</v>
+      <c r="CJ61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CK61" s="0"/>
       <c r="CL61" s="0"/>
       <c r="CM61" s="2"/>
       <c r="CN61" s="0"/>
-      <c r="CO61" s="80" t="s">
-        <v>1056</v>
+      <c r="CO61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CP61" s="0"/>
       <c r="CQ61" s="0"/>
       <c r="CR61" s="2"/>
       <c r="CS61" s="0"/>
-      <c r="CT61" s="80" t="s">
-        <v>1056</v>
+      <c r="CT61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CU61" s="0"/>
       <c r="CV61" s="0"/>
       <c r="CW61" s="2"/>
       <c r="CX61" s="0"/>
-      <c r="CY61" s="80" t="s">
-        <v>1056</v>
+      <c r="CY61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="CZ61" s="0"/>
       <c r="DA61" s="0"/>
       <c r="DB61" s="2"/>
       <c r="DC61" s="0"/>
-      <c r="DD61" s="80" t="s">
-        <v>1056</v>
+      <c r="DD61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="DE61" s="0"/>
       <c r="DF61" s="0"/>
       <c r="DG61" s="2"/>
       <c r="DH61" s="0"/>
-      <c r="DI61" s="80" t="s">
-        <v>1056</v>
+      <c r="DI61" s="79" t="s">
+        <v>1055</v>
       </c>
       <c r="DJ61" s="0"/>
       <c r="DK61" s="0"/>
@@ -65538,159 +65518,159 @@
     <row r="62" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0"/>
       <c r="B62" s="0"/>
-      <c r="C62" s="81" t="s">
-        <v>123</v>
+      <c r="C62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="D62" s="0"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
       <c r="G62" s="0"/>
-      <c r="H62" s="81" t="s">
-        <v>123</v>
+      <c r="H62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="I62" s="0"/>
       <c r="J62" s="0"/>
       <c r="K62" s="0"/>
       <c r="L62" s="0"/>
-      <c r="M62" s="81" t="s">
-        <v>123</v>
+      <c r="M62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="N62" s="0"/>
       <c r="O62" s="0"/>
       <c r="P62" s="0"/>
       <c r="Q62" s="0"/>
-      <c r="R62" s="81" t="s">
-        <v>123</v>
+      <c r="R62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="S62" s="0"/>
       <c r="T62" s="3"/>
       <c r="U62" s="0"/>
       <c r="V62" s="0"/>
-      <c r="W62" s="81" t="s">
-        <v>123</v>
+      <c r="W62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="X62" s="0"/>
       <c r="Y62" s="3"/>
       <c r="Z62" s="0"/>
       <c r="AA62" s="0"/>
-      <c r="AB62" s="81" t="s">
-        <v>123</v>
+      <c r="AB62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="AC62" s="0"/>
       <c r="AE62" s="0"/>
       <c r="AF62" s="0"/>
-      <c r="AG62" s="81" t="s">
-        <v>123</v>
+      <c r="AG62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="AH62" s="0"/>
       <c r="AJ62" s="0"/>
       <c r="AK62" s="0"/>
-      <c r="AL62" s="81" t="s">
-        <v>123</v>
+      <c r="AL62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="AM62" s="0"/>
       <c r="AN62" s="3"/>
       <c r="AO62" s="0"/>
       <c r="AP62" s="0"/>
-      <c r="AQ62" s="81" t="s">
-        <v>123</v>
+      <c r="AQ62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="AR62" s="0"/>
       <c r="AS62" s="0"/>
       <c r="AT62" s="0"/>
       <c r="AU62" s="0"/>
-      <c r="AV62" s="81" t="s">
-        <v>123</v>
+      <c r="AV62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="AW62" s="0"/>
       <c r="AY62" s="0"/>
       <c r="AZ62" s="0"/>
-      <c r="BA62" s="81" t="s">
-        <v>123</v>
+      <c r="BA62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="BB62" s="0"/>
       <c r="BC62" s="0"/>
       <c r="BD62" s="0"/>
       <c r="BE62" s="0"/>
-      <c r="BF62" s="81" t="s">
-        <v>123</v>
+      <c r="BF62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="BG62" s="0"/>
       <c r="BH62" s="0"/>
       <c r="BI62" s="0"/>
       <c r="BJ62" s="0"/>
-      <c r="BK62" s="81" t="s">
-        <v>123</v>
+      <c r="BK62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="BL62" s="0"/>
       <c r="BM62" s="0"/>
       <c r="BN62" s="0"/>
       <c r="BO62" s="0"/>
-      <c r="BP62" s="81" t="s">
-        <v>123</v>
+      <c r="BP62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="BQ62" s="0"/>
       <c r="BR62" s="0"/>
       <c r="BS62" s="0"/>
       <c r="BT62" s="0"/>
-      <c r="BU62" s="81" t="s">
-        <v>123</v>
+      <c r="BU62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="BV62" s="0"/>
       <c r="BW62" s="0"/>
       <c r="BX62" s="0"/>
       <c r="BY62" s="0"/>
-      <c r="BZ62" s="81" t="s">
-        <v>123</v>
+      <c r="BZ62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CA62" s="0"/>
       <c r="CB62" s="0"/>
       <c r="CC62" s="0"/>
       <c r="CD62" s="0"/>
-      <c r="CE62" s="81" t="s">
-        <v>123</v>
+      <c r="CE62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CF62" s="0"/>
       <c r="CG62" s="0"/>
       <c r="CH62" s="2"/>
       <c r="CI62" s="0"/>
-      <c r="CJ62" s="81" t="s">
-        <v>123</v>
+      <c r="CJ62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CK62" s="0"/>
       <c r="CL62" s="0"/>
       <c r="CM62" s="2"/>
       <c r="CN62" s="0"/>
-      <c r="CO62" s="81" t="s">
-        <v>123</v>
+      <c r="CO62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CP62" s="0"/>
       <c r="CQ62" s="0"/>
       <c r="CR62" s="2"/>
       <c r="CS62" s="0"/>
-      <c r="CT62" s="81" t="s">
-        <v>123</v>
+      <c r="CT62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CU62" s="0"/>
       <c r="CV62" s="0"/>
       <c r="CW62" s="2"/>
       <c r="CX62" s="0"/>
-      <c r="CY62" s="81" t="s">
-        <v>123</v>
+      <c r="CY62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="CZ62" s="0"/>
       <c r="DA62" s="0"/>
       <c r="DB62" s="2"/>
       <c r="DC62" s="0"/>
-      <c r="DD62" s="81" t="s">
-        <v>123</v>
+      <c r="DD62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="DE62" s="0"/>
       <c r="DF62" s="0"/>
       <c r="DG62" s="2"/>
       <c r="DH62" s="0"/>
-      <c r="DI62" s="81" t="s">
-        <v>123</v>
+      <c r="DI62" s="37" t="s">
+        <v>1056</v>
       </c>
       <c r="DJ62" s="0"/>
       <c r="DK62" s="0"/>
@@ -65698,480 +65678,320 @@
     <row r="63" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
-      <c r="C63" s="37" t="s">
+      <c r="C63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="D63" s="0"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
       <c r="G63" s="0"/>
-      <c r="H63" s="37" t="s">
+      <c r="H63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="I63" s="0"/>
       <c r="J63" s="0"/>
       <c r="K63" s="0"/>
       <c r="L63" s="0"/>
-      <c r="M63" s="37" t="s">
+      <c r="M63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="N63" s="0"/>
       <c r="O63" s="0"/>
       <c r="P63" s="0"/>
       <c r="Q63" s="0"/>
-      <c r="R63" s="37" t="s">
+      <c r="R63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="S63" s="0"/>
       <c r="T63" s="3"/>
       <c r="U63" s="0"/>
       <c r="V63" s="0"/>
-      <c r="W63" s="37" t="s">
+      <c r="W63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="X63" s="0"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="0"/>
       <c r="AA63" s="0"/>
-      <c r="AB63" s="37" t="s">
+      <c r="AB63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="AC63" s="0"/>
       <c r="AE63" s="0"/>
       <c r="AF63" s="0"/>
-      <c r="AG63" s="37" t="s">
+      <c r="AG63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="AH63" s="0"/>
       <c r="AJ63" s="0"/>
       <c r="AK63" s="0"/>
-      <c r="AL63" s="37" t="s">
+      <c r="AL63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="AM63" s="0"/>
       <c r="AN63" s="3"/>
       <c r="AO63" s="0"/>
       <c r="AP63" s="0"/>
-      <c r="AQ63" s="37" t="s">
+      <c r="AQ63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="AR63" s="0"/>
       <c r="AS63" s="0"/>
       <c r="AT63" s="0"/>
       <c r="AU63" s="0"/>
-      <c r="AV63" s="37" t="s">
+      <c r="AV63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="AW63" s="0"/>
       <c r="AY63" s="0"/>
       <c r="AZ63" s="0"/>
-      <c r="BA63" s="37" t="s">
+      <c r="BA63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="BB63" s="0"/>
       <c r="BC63" s="0"/>
       <c r="BD63" s="0"/>
       <c r="BE63" s="0"/>
-      <c r="BF63" s="37" t="s">
+      <c r="BF63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="BG63" s="0"/>
       <c r="BH63" s="0"/>
       <c r="BI63" s="0"/>
       <c r="BJ63" s="0"/>
-      <c r="BK63" s="37" t="s">
+      <c r="BK63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="BL63" s="0"/>
       <c r="BM63" s="0"/>
       <c r="BN63" s="0"/>
       <c r="BO63" s="0"/>
-      <c r="BP63" s="37" t="s">
+      <c r="BP63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="BQ63" s="0"/>
       <c r="BR63" s="0"/>
       <c r="BS63" s="0"/>
       <c r="BT63" s="0"/>
-      <c r="BU63" s="37" t="s">
+      <c r="BU63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="BV63" s="0"/>
       <c r="BW63" s="0"/>
       <c r="BX63" s="0"/>
       <c r="BY63" s="0"/>
-      <c r="BZ63" s="37" t="s">
+      <c r="BZ63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CA63" s="0"/>
       <c r="CB63" s="0"/>
       <c r="CC63" s="0"/>
       <c r="CD63" s="0"/>
-      <c r="CE63" s="37" t="s">
+      <c r="CE63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CF63" s="0"/>
       <c r="CG63" s="0"/>
       <c r="CH63" s="2"/>
       <c r="CI63" s="0"/>
-      <c r="CJ63" s="37" t="s">
+      <c r="CJ63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CK63" s="0"/>
       <c r="CL63" s="0"/>
       <c r="CM63" s="2"/>
       <c r="CN63" s="0"/>
-      <c r="CO63" s="37" t="s">
+      <c r="CO63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CP63" s="0"/>
       <c r="CQ63" s="0"/>
       <c r="CR63" s="2"/>
       <c r="CS63" s="0"/>
-      <c r="CT63" s="37" t="s">
+      <c r="CT63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CU63" s="0"/>
       <c r="CV63" s="0"/>
       <c r="CW63" s="2"/>
       <c r="CX63" s="0"/>
-      <c r="CY63" s="37" t="s">
+      <c r="CY63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="CZ63" s="0"/>
       <c r="DA63" s="0"/>
       <c r="DB63" s="2"/>
       <c r="DC63" s="0"/>
-      <c r="DD63" s="37" t="s">
+      <c r="DD63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="DE63" s="0"/>
       <c r="DF63" s="0"/>
       <c r="DG63" s="2"/>
       <c r="DH63" s="0"/>
-      <c r="DI63" s="37" t="s">
+      <c r="DI63" s="36" t="s">
         <v>1057</v>
       </c>
       <c r="DJ63" s="0"/>
       <c r="DK63" s="0"/>
     </row>
     <row r="64" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0"/>
-      <c r="B64" s="0"/>
-      <c r="C64" s="36" t="s">
+      <c r="C64" s="47" t="s">
         <v>1058</v>
       </c>
       <c r="D64" s="0"/>
       <c r="E64" s="0"/>
       <c r="F64" s="0"/>
       <c r="G64" s="0"/>
-      <c r="H64" s="36" t="s">
-        <v>1059</v>
+      <c r="H64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="I64" s="0"/>
       <c r="J64" s="0"/>
       <c r="K64" s="0"/>
       <c r="L64" s="0"/>
-      <c r="M64" s="36" t="s">
-        <v>1059</v>
+      <c r="M64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="N64" s="0"/>
       <c r="O64" s="0"/>
       <c r="P64" s="0"/>
       <c r="Q64" s="0"/>
-      <c r="R64" s="36" t="s">
-        <v>1059</v>
+      <c r="R64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="S64" s="0"/>
       <c r="T64" s="3"/>
       <c r="U64" s="0"/>
       <c r="V64" s="0"/>
-      <c r="W64" s="36" t="s">
-        <v>1059</v>
+      <c r="W64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="X64" s="0"/>
       <c r="Y64" s="3"/>
       <c r="Z64" s="0"/>
       <c r="AA64" s="0"/>
-      <c r="AB64" s="36" t="s">
-        <v>1059</v>
+      <c r="AB64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="AC64" s="0"/>
       <c r="AE64" s="0"/>
       <c r="AF64" s="0"/>
-      <c r="AG64" s="36" t="s">
-        <v>1059</v>
+      <c r="AG64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="AH64" s="0"/>
       <c r="AJ64" s="0"/>
       <c r="AK64" s="0"/>
-      <c r="AL64" s="36" t="s">
-        <v>1059</v>
+      <c r="AL64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="AM64" s="0"/>
       <c r="AN64" s="3"/>
       <c r="AO64" s="0"/>
       <c r="AP64" s="0"/>
-      <c r="AQ64" s="36" t="s">
-        <v>1059</v>
+      <c r="AQ64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="AR64" s="0"/>
       <c r="AS64" s="0"/>
       <c r="AT64" s="0"/>
       <c r="AU64" s="0"/>
-      <c r="AV64" s="36" t="s">
-        <v>1059</v>
+      <c r="AV64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="AW64" s="0"/>
       <c r="AY64" s="0"/>
       <c r="AZ64" s="0"/>
-      <c r="BA64" s="36" t="s">
-        <v>1059</v>
+      <c r="BA64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="BB64" s="0"/>
       <c r="BC64" s="0"/>
       <c r="BD64" s="0"/>
       <c r="BE64" s="0"/>
-      <c r="BF64" s="36" t="s">
-        <v>1059</v>
+      <c r="BF64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="BG64" s="0"/>
       <c r="BH64" s="0"/>
       <c r="BI64" s="0"/>
       <c r="BJ64" s="0"/>
-      <c r="BK64" s="36" t="s">
-        <v>1059</v>
+      <c r="BK64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="BL64" s="0"/>
       <c r="BM64" s="0"/>
       <c r="BN64" s="0"/>
       <c r="BO64" s="0"/>
-      <c r="BP64" s="36" t="s">
-        <v>1059</v>
+      <c r="BP64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="BQ64" s="0"/>
       <c r="BR64" s="0"/>
       <c r="BS64" s="0"/>
       <c r="BT64" s="0"/>
-      <c r="BU64" s="36" t="s">
-        <v>1059</v>
+      <c r="BU64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="BV64" s="0"/>
       <c r="BW64" s="0"/>
       <c r="BX64" s="0"/>
       <c r="BY64" s="0"/>
-      <c r="BZ64" s="36" t="s">
-        <v>1059</v>
+      <c r="BZ64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CA64" s="0"/>
       <c r="CB64" s="0"/>
       <c r="CC64" s="0"/>
       <c r="CD64" s="0"/>
-      <c r="CE64" s="36" t="s">
-        <v>1059</v>
+      <c r="CE64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CF64" s="0"/>
       <c r="CG64" s="0"/>
       <c r="CH64" s="2"/>
       <c r="CI64" s="0"/>
-      <c r="CJ64" s="36" t="s">
-        <v>1059</v>
+      <c r="CJ64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CK64" s="0"/>
       <c r="CL64" s="0"/>
       <c r="CM64" s="2"/>
       <c r="CN64" s="0"/>
-      <c r="CO64" s="36" t="s">
-        <v>1059</v>
+      <c r="CO64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CP64" s="0"/>
       <c r="CQ64" s="0"/>
       <c r="CR64" s="2"/>
       <c r="CS64" s="0"/>
-      <c r="CT64" s="36" t="s">
-        <v>1059</v>
+      <c r="CT64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CU64" s="0"/>
       <c r="CV64" s="0"/>
       <c r="CW64" s="2"/>
       <c r="CX64" s="0"/>
-      <c r="CY64" s="36" t="s">
-        <v>1059</v>
+      <c r="CY64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="CZ64" s="0"/>
       <c r="DA64" s="0"/>
       <c r="DB64" s="2"/>
       <c r="DC64" s="0"/>
-      <c r="DD64" s="36" t="s">
-        <v>1059</v>
+      <c r="DD64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="DE64" s="0"/>
       <c r="DF64" s="0"/>
       <c r="DG64" s="2"/>
       <c r="DH64" s="0"/>
-      <c r="DI64" s="36" t="s">
-        <v>1059</v>
+      <c r="DI64" s="47" t="s">
+        <v>1058</v>
       </c>
       <c r="DJ64" s="0"/>
       <c r="DK64" s="0"/>
-    </row>
-    <row r="65" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D65" s="0"/>
-      <c r="E65" s="0"/>
-      <c r="F65" s="0"/>
-      <c r="G65" s="0"/>
-      <c r="H65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="I65" s="0"/>
-      <c r="J65" s="0"/>
-      <c r="K65" s="0"/>
-      <c r="L65" s="0"/>
-      <c r="M65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="N65" s="0"/>
-      <c r="O65" s="0"/>
-      <c r="P65" s="0"/>
-      <c r="Q65" s="0"/>
-      <c r="R65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="S65" s="0"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="0"/>
-      <c r="V65" s="0"/>
-      <c r="W65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="X65" s="0"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="0"/>
-      <c r="AA65" s="0"/>
-      <c r="AB65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="AC65" s="0"/>
-      <c r="AE65" s="0"/>
-      <c r="AF65" s="0"/>
-      <c r="AG65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="AH65" s="0"/>
-      <c r="AJ65" s="0"/>
-      <c r="AK65" s="0"/>
-      <c r="AL65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="AM65" s="0"/>
-      <c r="AN65" s="3"/>
-      <c r="AO65" s="0"/>
-      <c r="AP65" s="0"/>
-      <c r="AQ65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="AR65" s="0"/>
-      <c r="AS65" s="0"/>
-      <c r="AT65" s="0"/>
-      <c r="AU65" s="0"/>
-      <c r="AV65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="AW65" s="0"/>
-      <c r="AY65" s="0"/>
-      <c r="AZ65" s="0"/>
-      <c r="BA65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BB65" s="0"/>
-      <c r="BC65" s="0"/>
-      <c r="BD65" s="0"/>
-      <c r="BE65" s="0"/>
-      <c r="BF65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BG65" s="0"/>
-      <c r="BH65" s="0"/>
-      <c r="BI65" s="0"/>
-      <c r="BJ65" s="0"/>
-      <c r="BK65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BL65" s="0"/>
-      <c r="BM65" s="0"/>
-      <c r="BN65" s="0"/>
-      <c r="BO65" s="0"/>
-      <c r="BP65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BQ65" s="0"/>
-      <c r="BR65" s="0"/>
-      <c r="BS65" s="0"/>
-      <c r="BT65" s="0"/>
-      <c r="BU65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="BV65" s="0"/>
-      <c r="BW65" s="0"/>
-      <c r="BX65" s="0"/>
-      <c r="BY65" s="0"/>
-      <c r="BZ65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CA65" s="0"/>
-      <c r="CB65" s="0"/>
-      <c r="CC65" s="0"/>
-      <c r="CD65" s="0"/>
-      <c r="CE65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CF65" s="0"/>
-      <c r="CG65" s="0"/>
-      <c r="CH65" s="2"/>
-      <c r="CI65" s="0"/>
-      <c r="CJ65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CK65" s="0"/>
-      <c r="CL65" s="0"/>
-      <c r="CM65" s="2"/>
-      <c r="CN65" s="0"/>
-      <c r="CO65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CP65" s="0"/>
-      <c r="CQ65" s="0"/>
-      <c r="CR65" s="2"/>
-      <c r="CS65" s="0"/>
-      <c r="CT65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CU65" s="0"/>
-      <c r="CV65" s="0"/>
-      <c r="CW65" s="2"/>
-      <c r="CX65" s="0"/>
-      <c r="CY65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="CZ65" s="0"/>
-      <c r="DA65" s="0"/>
-      <c r="DB65" s="2"/>
-      <c r="DC65" s="0"/>
-      <c r="DD65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="DE65" s="0"/>
-      <c r="DF65" s="0"/>
-      <c r="DG65" s="2"/>
-      <c r="DH65" s="0"/>
-      <c r="DI65" s="47" t="s">
-        <v>1060</v>
-      </c>
-      <c r="DJ65" s="0"/>
-      <c r="DK65" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="269">

</xml_diff>

<commit_message>
change administrator to ADMIN
</commit_message>
<xml_diff>
--- a/flask-backend/Rack Info-201703.xlsx
+++ b/flask-backend/Rack Info-201703.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1060">
   <si>
     <t xml:space="preserve">R00 - R11003</t>
   </si>
@@ -3374,6 +3374,9 @@
   </si>
   <si>
     <t xml:space="preserve">S14057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMIN</t>
   </si>
   <si>
     <t xml:space="preserve">Administrator</t>
@@ -7442,7 +7445,7 @@
   <dimension ref="1:64"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -62132,348 +62135,348 @@
       </c>
       <c r="F51" s="72"/>
       <c r="H51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="K51" s="72"/>
       <c r="M51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="P51" s="72"/>
       <c r="R51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="U51" s="72"/>
       <c r="W51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="Z51" s="72"/>
       <c r="AB51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="AE51" s="72"/>
       <c r="AG51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="AJ51" s="72"/>
       <c r="AL51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="AO51" s="72"/>
       <c r="AQ51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="AT51" s="72"/>
       <c r="AV51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="AY51" s="72"/>
       <c r="BA51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="BD51" s="72"/>
       <c r="BF51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="BI51" s="72"/>
       <c r="BK51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="BN51" s="72"/>
       <c r="BP51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="BS51" s="72"/>
       <c r="BU51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="BX51" s="72"/>
       <c r="BZ51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="CC51" s="72"/>
       <c r="CE51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="CH51" s="72"/>
       <c r="CJ51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="CM51" s="72"/>
       <c r="CO51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="CR51" s="72"/>
       <c r="CT51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="CW51" s="72"/>
       <c r="CY51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="DB51" s="72"/>
       <c r="DD51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="DG51" s="72"/>
       <c r="DI51" s="46" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="52" s="73" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="F52" s="74"/>
       <c r="H52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="K52" s="74"/>
       <c r="M52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="P52" s="74"/>
       <c r="R52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="T52" s="8"/>
       <c r="U52" s="74"/>
       <c r="W52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="Y52" s="8"/>
       <c r="Z52" s="74"/>
       <c r="AB52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AE52" s="74"/>
       <c r="AG52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AJ52" s="74"/>
       <c r="AL52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AN52" s="8"/>
       <c r="AO52" s="74"/>
       <c r="AQ52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AT52" s="74"/>
       <c r="AV52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="AY52" s="74"/>
       <c r="BA52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="BD52" s="74"/>
       <c r="BF52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="BI52" s="74"/>
       <c r="BK52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="BN52" s="74"/>
       <c r="BP52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="BS52" s="74"/>
       <c r="BU52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="BX52" s="74"/>
       <c r="BZ52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="CC52" s="74"/>
       <c r="CE52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="CH52" s="74"/>
       <c r="CJ52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="CM52" s="74"/>
       <c r="CO52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="CR52" s="74"/>
       <c r="CT52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="CW52" s="74"/>
       <c r="CY52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="DB52" s="74"/>
       <c r="DD52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="DG52" s="74"/>
       <c r="DI52" s="32" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0"/>
       <c r="B53" s="0"/>
       <c r="C53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
       <c r="G53" s="0"/>
       <c r="H53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="I53" s="0"/>
       <c r="J53" s="0"/>
       <c r="K53" s="0"/>
       <c r="L53" s="0"/>
       <c r="M53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="N53" s="0"/>
       <c r="O53" s="0"/>
       <c r="P53" s="0"/>
       <c r="Q53" s="0"/>
       <c r="R53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="S53" s="0"/>
       <c r="T53" s="3"/>
       <c r="U53" s="0"/>
       <c r="V53" s="0"/>
       <c r="W53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="X53" s="0"/>
       <c r="Y53" s="3"/>
       <c r="Z53" s="0"/>
       <c r="AA53" s="0"/>
       <c r="AB53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AC53" s="0"/>
       <c r="AD53" s="1"/>
       <c r="AE53" s="0"/>
       <c r="AF53" s="0"/>
       <c r="AG53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AH53" s="0"/>
       <c r="AI53" s="1"/>
       <c r="AJ53" s="0"/>
       <c r="AK53" s="0"/>
       <c r="AL53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AM53" s="0"/>
       <c r="AN53" s="3"/>
       <c r="AO53" s="0"/>
       <c r="AP53" s="0"/>
       <c r="AQ53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AR53" s="0"/>
       <c r="AS53" s="0"/>
       <c r="AT53" s="0"/>
       <c r="AU53" s="0"/>
       <c r="AV53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="AW53" s="0"/>
       <c r="AX53" s="1"/>
       <c r="AY53" s="0"/>
       <c r="AZ53" s="0"/>
       <c r="BA53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="BB53" s="0"/>
       <c r="BC53" s="0"/>
       <c r="BD53" s="0"/>
       <c r="BE53" s="0"/>
       <c r="BF53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="BG53" s="0"/>
       <c r="BH53" s="0"/>
       <c r="BI53" s="0"/>
       <c r="BJ53" s="0"/>
       <c r="BK53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="BL53" s="0"/>
       <c r="BM53" s="0"/>
       <c r="BN53" s="0"/>
       <c r="BO53" s="0"/>
       <c r="BP53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="BQ53" s="0"/>
       <c r="BR53" s="0"/>
       <c r="BS53" s="0"/>
       <c r="BT53" s="0"/>
       <c r="BU53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="BV53" s="0"/>
       <c r="BW53" s="0"/>
       <c r="BX53" s="0"/>
       <c r="BY53" s="0"/>
       <c r="BZ53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CA53" s="0"/>
       <c r="CB53" s="0"/>
       <c r="CC53" s="0"/>
       <c r="CD53" s="0"/>
       <c r="CE53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CF53" s="0"/>
       <c r="CG53" s="0"/>
       <c r="CH53" s="2"/>
       <c r="CI53" s="0"/>
       <c r="CJ53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CK53" s="0"/>
       <c r="CL53" s="0"/>
       <c r="CM53" s="2"/>
       <c r="CN53" s="0"/>
       <c r="CO53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CP53" s="0"/>
       <c r="CQ53" s="0"/>
       <c r="CR53" s="2"/>
       <c r="CS53" s="0"/>
       <c r="CT53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CU53" s="0"/>
       <c r="CV53" s="0"/>
       <c r="CW53" s="2"/>
       <c r="CX53" s="0"/>
       <c r="CY53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="CZ53" s="0"/>
       <c r="DA53" s="0"/>
       <c r="DB53" s="2"/>
       <c r="DC53" s="0"/>
       <c r="DD53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="DE53" s="0"/>
       <c r="DF53" s="0"/>
       <c r="DG53" s="2"/>
       <c r="DH53" s="0"/>
       <c r="DI53" s="75" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="DJ53" s="0"/>
       <c r="DK53" s="0"/>
@@ -63391,161 +63394,161 @@
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
       <c r="C54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="D54" s="0"/>
       <c r="E54" s="0"/>
       <c r="F54" s="0"/>
       <c r="G54" s="0"/>
       <c r="H54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="I54" s="0"/>
       <c r="J54" s="0"/>
       <c r="K54" s="0"/>
       <c r="L54" s="0"/>
       <c r="M54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="N54" s="0"/>
       <c r="O54" s="0"/>
       <c r="P54" s="0"/>
       <c r="Q54" s="0"/>
       <c r="R54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="S54" s="0"/>
       <c r="T54" s="3"/>
       <c r="U54" s="0"/>
       <c r="V54" s="0"/>
       <c r="W54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="X54" s="0"/>
       <c r="Y54" s="3"/>
       <c r="Z54" s="0"/>
       <c r="AA54" s="0"/>
       <c r="AB54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AC54" s="0"/>
       <c r="AD54" s="1"/>
       <c r="AE54" s="0"/>
       <c r="AF54" s="0"/>
       <c r="AG54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AH54" s="0"/>
       <c r="AI54" s="1"/>
       <c r="AJ54" s="0"/>
       <c r="AK54" s="0"/>
       <c r="AL54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AM54" s="0"/>
       <c r="AN54" s="3"/>
       <c r="AO54" s="0"/>
       <c r="AP54" s="0"/>
       <c r="AQ54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AR54" s="0"/>
       <c r="AS54" s="0"/>
       <c r="AT54" s="0"/>
       <c r="AU54" s="0"/>
       <c r="AV54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="AW54" s="0"/>
       <c r="AX54" s="1"/>
       <c r="AY54" s="0"/>
       <c r="AZ54" s="0"/>
       <c r="BA54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="BB54" s="0"/>
       <c r="BC54" s="0"/>
       <c r="BD54" s="0"/>
       <c r="BE54" s="0"/>
       <c r="BF54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="BG54" s="0"/>
       <c r="BH54" s="0"/>
       <c r="BI54" s="0"/>
       <c r="BJ54" s="0"/>
       <c r="BK54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="BL54" s="0"/>
       <c r="BM54" s="0"/>
       <c r="BN54" s="0"/>
       <c r="BO54" s="0"/>
       <c r="BP54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="BQ54" s="0"/>
       <c r="BR54" s="0"/>
       <c r="BS54" s="0"/>
       <c r="BT54" s="0"/>
       <c r="BU54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="BV54" s="0"/>
       <c r="BW54" s="0"/>
       <c r="BX54" s="0"/>
       <c r="BY54" s="0"/>
       <c r="BZ54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CA54" s="0"/>
       <c r="CB54" s="0"/>
       <c r="CC54" s="0"/>
       <c r="CD54" s="0"/>
       <c r="CE54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CF54" s="0"/>
       <c r="CG54" s="0"/>
       <c r="CH54" s="2"/>
       <c r="CI54" s="0"/>
       <c r="CJ54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CK54" s="0"/>
       <c r="CL54" s="0"/>
       <c r="CM54" s="2"/>
       <c r="CN54" s="0"/>
       <c r="CO54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CP54" s="0"/>
       <c r="CQ54" s="0"/>
       <c r="CR54" s="2"/>
       <c r="CS54" s="0"/>
       <c r="CT54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CU54" s="0"/>
       <c r="CV54" s="0"/>
       <c r="CW54" s="2"/>
       <c r="CX54" s="0"/>
       <c r="CY54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="CZ54" s="0"/>
       <c r="DA54" s="0"/>
       <c r="DB54" s="2"/>
       <c r="DC54" s="0"/>
       <c r="DD54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="DE54" s="0"/>
       <c r="DF54" s="0"/>
       <c r="DG54" s="2"/>
       <c r="DH54" s="0"/>
       <c r="DI54" s="44" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="DJ54" s="0"/>
       <c r="DK54" s="0"/>
@@ -64461,256 +64464,256 @@
     </row>
     <row r="55" s="73" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F55" s="74"/>
       <c r="H55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="K55" s="74"/>
       <c r="M55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="P55" s="74"/>
       <c r="R55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="T55" s="8"/>
       <c r="U55" s="74"/>
       <c r="W55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="Y55" s="8"/>
       <c r="Z55" s="74"/>
       <c r="AB55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="AE55" s="74"/>
       <c r="AG55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="AJ55" s="74"/>
       <c r="AL55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="AN55" s="8"/>
       <c r="AO55" s="74"/>
       <c r="AQ55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="AT55" s="74"/>
       <c r="AV55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="AY55" s="74"/>
       <c r="BA55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="BD55" s="74"/>
       <c r="BF55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="BI55" s="74"/>
       <c r="BK55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="BN55" s="74"/>
       <c r="BP55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="BS55" s="74"/>
       <c r="BU55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="BX55" s="74"/>
       <c r="BZ55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="CC55" s="74"/>
       <c r="CE55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="CH55" s="74"/>
       <c r="CJ55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="CM55" s="74"/>
       <c r="CO55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="CR55" s="74"/>
       <c r="CT55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="CW55" s="74"/>
       <c r="CY55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="DB55" s="74"/>
       <c r="DD55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="DG55" s="74"/>
       <c r="DI55" s="76" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
       <c r="B56" s="0"/>
       <c r="C56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="D56" s="0"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
       <c r="G56" s="0"/>
       <c r="H56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="I56" s="0"/>
       <c r="J56" s="0"/>
       <c r="K56" s="0"/>
       <c r="L56" s="0"/>
       <c r="M56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="N56" s="0"/>
       <c r="O56" s="0"/>
       <c r="P56" s="0"/>
       <c r="Q56" s="0"/>
       <c r="R56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="S56" s="0"/>
       <c r="T56" s="3"/>
       <c r="U56" s="0"/>
       <c r="V56" s="0"/>
       <c r="W56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="X56" s="0"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="0"/>
       <c r="AA56" s="0"/>
       <c r="AB56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="AC56" s="0"/>
       <c r="AE56" s="0"/>
       <c r="AF56" s="0"/>
       <c r="AG56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="AH56" s="0"/>
       <c r="AJ56" s="0"/>
       <c r="AK56" s="0"/>
       <c r="AL56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="AM56" s="0"/>
       <c r="AN56" s="3"/>
       <c r="AO56" s="0"/>
       <c r="AP56" s="0"/>
       <c r="AQ56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="AR56" s="0"/>
       <c r="AS56" s="0"/>
       <c r="AT56" s="0"/>
       <c r="AU56" s="0"/>
       <c r="AV56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="AW56" s="0"/>
       <c r="AY56" s="0"/>
       <c r="AZ56" s="0"/>
       <c r="BA56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="BB56" s="0"/>
       <c r="BC56" s="0"/>
       <c r="BD56" s="0"/>
       <c r="BE56" s="0"/>
       <c r="BF56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="BG56" s="0"/>
       <c r="BH56" s="0"/>
       <c r="BI56" s="0"/>
       <c r="BJ56" s="0"/>
       <c r="BK56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="BL56" s="0"/>
       <c r="BM56" s="0"/>
       <c r="BN56" s="0"/>
       <c r="BO56" s="0"/>
       <c r="BP56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="BQ56" s="0"/>
       <c r="BR56" s="0"/>
       <c r="BS56" s="0"/>
       <c r="BT56" s="0"/>
       <c r="BU56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="BV56" s="0"/>
       <c r="BW56" s="0"/>
       <c r="BX56" s="0"/>
       <c r="BY56" s="0"/>
       <c r="BZ56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CA56" s="0"/>
       <c r="CB56" s="0"/>
       <c r="CC56" s="0"/>
       <c r="CD56" s="0"/>
       <c r="CE56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CF56" s="0"/>
       <c r="CG56" s="0"/>
       <c r="CH56" s="2"/>
       <c r="CI56" s="0"/>
       <c r="CJ56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CK56" s="0"/>
       <c r="CL56" s="0"/>
       <c r="CM56" s="2"/>
       <c r="CN56" s="0"/>
       <c r="CO56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CP56" s="0"/>
       <c r="CQ56" s="0"/>
       <c r="CR56" s="2"/>
       <c r="CS56" s="0"/>
       <c r="CT56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CU56" s="0"/>
       <c r="CV56" s="0"/>
       <c r="CW56" s="2"/>
       <c r="CX56" s="0"/>
       <c r="CY56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="CZ56" s="0"/>
       <c r="DA56" s="0"/>
       <c r="DB56" s="2"/>
       <c r="DC56" s="0"/>
       <c r="DD56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="DE56" s="0"/>
       <c r="DF56" s="0"/>
       <c r="DG56" s="2"/>
       <c r="DH56" s="0"/>
       <c r="DI56" s="58" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="DJ56" s="0"/>
       <c r="DK56" s="0"/>
@@ -64719,158 +64722,158 @@
       <c r="A57" s="0"/>
       <c r="B57" s="0"/>
       <c r="C57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="D57" s="0"/>
       <c r="E57" s="0"/>
       <c r="F57" s="0"/>
       <c r="G57" s="0"/>
       <c r="H57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="I57" s="0"/>
       <c r="J57" s="0"/>
       <c r="K57" s="0"/>
       <c r="L57" s="0"/>
       <c r="M57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="N57" s="0"/>
       <c r="O57" s="0"/>
       <c r="P57" s="0"/>
       <c r="Q57" s="0"/>
       <c r="R57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="S57" s="0"/>
       <c r="T57" s="3"/>
       <c r="U57" s="0"/>
       <c r="V57" s="0"/>
       <c r="W57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="X57" s="0"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="0"/>
       <c r="AA57" s="0"/>
       <c r="AB57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="AC57" s="0"/>
       <c r="AE57" s="0"/>
       <c r="AF57" s="0"/>
       <c r="AG57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="AH57" s="0"/>
       <c r="AJ57" s="0"/>
       <c r="AK57" s="0"/>
       <c r="AL57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="AM57" s="0"/>
       <c r="AN57" s="3"/>
       <c r="AO57" s="0"/>
       <c r="AP57" s="0"/>
       <c r="AQ57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="AR57" s="0"/>
       <c r="AS57" s="0"/>
       <c r="AT57" s="0"/>
       <c r="AU57" s="0"/>
       <c r="AV57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="AW57" s="0"/>
       <c r="AY57" s="0"/>
       <c r="AZ57" s="0"/>
       <c r="BA57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="BB57" s="0"/>
       <c r="BC57" s="0"/>
       <c r="BD57" s="0"/>
       <c r="BE57" s="0"/>
       <c r="BF57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="BG57" s="0"/>
       <c r="BH57" s="0"/>
       <c r="BI57" s="0"/>
       <c r="BJ57" s="0"/>
       <c r="BK57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="BL57" s="0"/>
       <c r="BM57" s="0"/>
       <c r="BN57" s="0"/>
       <c r="BO57" s="0"/>
       <c r="BP57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="BQ57" s="0"/>
       <c r="BR57" s="0"/>
       <c r="BS57" s="0"/>
       <c r="BT57" s="0"/>
       <c r="BU57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="BV57" s="0"/>
       <c r="BW57" s="0"/>
       <c r="BX57" s="0"/>
       <c r="BY57" s="0"/>
       <c r="BZ57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CA57" s="0"/>
       <c r="CB57" s="0"/>
       <c r="CC57" s="0"/>
       <c r="CD57" s="0"/>
       <c r="CE57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CF57" s="0"/>
       <c r="CG57" s="0"/>
       <c r="CH57" s="2"/>
       <c r="CI57" s="0"/>
       <c r="CJ57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CK57" s="0"/>
       <c r="CL57" s="0"/>
       <c r="CM57" s="2"/>
       <c r="CN57" s="0"/>
       <c r="CO57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CP57" s="0"/>
       <c r="CQ57" s="0"/>
       <c r="CR57" s="2"/>
       <c r="CS57" s="0"/>
       <c r="CT57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CU57" s="0"/>
       <c r="CV57" s="0"/>
       <c r="CW57" s="2"/>
       <c r="CX57" s="0"/>
       <c r="CY57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="CZ57" s="0"/>
       <c r="DA57" s="0"/>
       <c r="DB57" s="2"/>
       <c r="DC57" s="0"/>
       <c r="DD57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="DE57" s="0"/>
       <c r="DF57" s="0"/>
       <c r="DG57" s="2"/>
       <c r="DH57" s="0"/>
       <c r="DI57" s="45" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="DJ57" s="0"/>
       <c r="DK57" s="0"/>
@@ -64879,158 +64882,158 @@
       <c r="A58" s="0"/>
       <c r="B58" s="0"/>
       <c r="C58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="D58" s="0"/>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
       <c r="G58" s="0"/>
       <c r="H58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="I58" s="0"/>
       <c r="J58" s="0"/>
       <c r="K58" s="0"/>
       <c r="L58" s="0"/>
       <c r="M58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="N58" s="0"/>
       <c r="O58" s="0"/>
       <c r="P58" s="0"/>
       <c r="Q58" s="0"/>
       <c r="R58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="S58" s="0"/>
       <c r="T58" s="3"/>
       <c r="U58" s="0"/>
       <c r="V58" s="0"/>
       <c r="W58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="X58" s="0"/>
       <c r="Y58" s="3"/>
       <c r="Z58" s="0"/>
       <c r="AA58" s="0"/>
       <c r="AB58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AC58" s="0"/>
       <c r="AE58" s="0"/>
       <c r="AF58" s="0"/>
       <c r="AG58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AH58" s="0"/>
       <c r="AJ58" s="0"/>
       <c r="AK58" s="0"/>
       <c r="AL58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AM58" s="0"/>
       <c r="AN58" s="3"/>
       <c r="AO58" s="0"/>
       <c r="AP58" s="0"/>
       <c r="AQ58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AR58" s="0"/>
       <c r="AS58" s="0"/>
       <c r="AT58" s="0"/>
       <c r="AU58" s="0"/>
       <c r="AV58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="AW58" s="0"/>
       <c r="AY58" s="0"/>
       <c r="AZ58" s="0"/>
       <c r="BA58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="BB58" s="0"/>
       <c r="BC58" s="0"/>
       <c r="BD58" s="0"/>
       <c r="BE58" s="0"/>
       <c r="BF58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="BG58" s="0"/>
       <c r="BH58" s="0"/>
       <c r="BI58" s="0"/>
       <c r="BJ58" s="0"/>
       <c r="BK58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="BL58" s="0"/>
       <c r="BM58" s="0"/>
       <c r="BN58" s="0"/>
       <c r="BO58" s="0"/>
       <c r="BP58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="BQ58" s="0"/>
       <c r="BR58" s="0"/>
       <c r="BS58" s="0"/>
       <c r="BT58" s="0"/>
       <c r="BU58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="BV58" s="0"/>
       <c r="BW58" s="0"/>
       <c r="BX58" s="0"/>
       <c r="BY58" s="0"/>
       <c r="BZ58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CA58" s="0"/>
       <c r="CB58" s="0"/>
       <c r="CC58" s="0"/>
       <c r="CD58" s="0"/>
       <c r="CE58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CF58" s="0"/>
       <c r="CG58" s="0"/>
       <c r="CH58" s="2"/>
       <c r="CI58" s="0"/>
       <c r="CJ58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CK58" s="0"/>
       <c r="CL58" s="0"/>
       <c r="CM58" s="2"/>
       <c r="CN58" s="0"/>
       <c r="CO58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CP58" s="0"/>
       <c r="CQ58" s="0"/>
       <c r="CR58" s="2"/>
       <c r="CS58" s="0"/>
       <c r="CT58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CU58" s="0"/>
       <c r="CV58" s="0"/>
       <c r="CW58" s="2"/>
       <c r="CX58" s="0"/>
       <c r="CY58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="CZ58" s="0"/>
       <c r="DA58" s="0"/>
       <c r="DB58" s="2"/>
       <c r="DC58" s="0"/>
       <c r="DD58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="DE58" s="0"/>
       <c r="DF58" s="0"/>
       <c r="DG58" s="2"/>
       <c r="DH58" s="0"/>
       <c r="DI58" s="77" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="DJ58" s="0"/>
       <c r="DK58" s="0"/>
@@ -65039,158 +65042,158 @@
       <c r="A59" s="0"/>
       <c r="B59" s="0"/>
       <c r="C59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="D59" s="0"/>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
       <c r="G59" s="0"/>
       <c r="H59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="I59" s="0"/>
       <c r="J59" s="0"/>
       <c r="K59" s="0"/>
       <c r="L59" s="0"/>
       <c r="M59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="N59" s="0"/>
       <c r="O59" s="0"/>
       <c r="P59" s="0"/>
       <c r="Q59" s="0"/>
       <c r="R59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="S59" s="0"/>
       <c r="T59" s="3"/>
       <c r="U59" s="0"/>
       <c r="V59" s="0"/>
       <c r="W59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="X59" s="0"/>
       <c r="Y59" s="3"/>
       <c r="Z59" s="0"/>
       <c r="AA59" s="0"/>
       <c r="AB59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="AC59" s="0"/>
       <c r="AE59" s="0"/>
       <c r="AF59" s="0"/>
       <c r="AG59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="AH59" s="0"/>
       <c r="AJ59" s="0"/>
       <c r="AK59" s="0"/>
       <c r="AL59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="AM59" s="0"/>
       <c r="AN59" s="3"/>
       <c r="AO59" s="0"/>
       <c r="AP59" s="0"/>
       <c r="AQ59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="AR59" s="0"/>
       <c r="AS59" s="0"/>
       <c r="AT59" s="0"/>
       <c r="AU59" s="0"/>
       <c r="AV59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="AW59" s="0"/>
       <c r="AY59" s="0"/>
       <c r="AZ59" s="0"/>
       <c r="BA59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="BB59" s="0"/>
       <c r="BC59" s="0"/>
       <c r="BD59" s="0"/>
       <c r="BE59" s="0"/>
       <c r="BF59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="BG59" s="0"/>
       <c r="BH59" s="0"/>
       <c r="BI59" s="0"/>
       <c r="BJ59" s="0"/>
       <c r="BK59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="BL59" s="0"/>
       <c r="BM59" s="0"/>
       <c r="BN59" s="0"/>
       <c r="BO59" s="0"/>
       <c r="BP59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="BQ59" s="0"/>
       <c r="BR59" s="0"/>
       <c r="BS59" s="0"/>
       <c r="BT59" s="0"/>
       <c r="BU59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="BV59" s="0"/>
       <c r="BW59" s="0"/>
       <c r="BX59" s="0"/>
       <c r="BY59" s="0"/>
       <c r="BZ59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CA59" s="0"/>
       <c r="CB59" s="0"/>
       <c r="CC59" s="0"/>
       <c r="CD59" s="0"/>
       <c r="CE59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CF59" s="0"/>
       <c r="CG59" s="0"/>
       <c r="CH59" s="2"/>
       <c r="CI59" s="0"/>
       <c r="CJ59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CK59" s="0"/>
       <c r="CL59" s="0"/>
       <c r="CM59" s="2"/>
       <c r="CN59" s="0"/>
       <c r="CO59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CP59" s="0"/>
       <c r="CQ59" s="0"/>
       <c r="CR59" s="2"/>
       <c r="CS59" s="0"/>
       <c r="CT59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CU59" s="0"/>
       <c r="CV59" s="0"/>
       <c r="CW59" s="2"/>
       <c r="CX59" s="0"/>
       <c r="CY59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="CZ59" s="0"/>
       <c r="DA59" s="0"/>
       <c r="DB59" s="2"/>
       <c r="DC59" s="0"/>
       <c r="DD59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="DE59" s="0"/>
       <c r="DF59" s="0"/>
       <c r="DG59" s="2"/>
       <c r="DH59" s="0"/>
       <c r="DI59" s="43" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="DJ59" s="0"/>
       <c r="DK59" s="0"/>
@@ -65199,158 +65202,158 @@
       <c r="A60" s="0"/>
       <c r="B60" s="0"/>
       <c r="C60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="D60" s="0"/>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
       <c r="G60" s="0"/>
       <c r="H60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="I60" s="0"/>
       <c r="J60" s="0"/>
       <c r="K60" s="0"/>
       <c r="L60" s="0"/>
       <c r="M60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="N60" s="0"/>
       <c r="O60" s="0"/>
       <c r="P60" s="0"/>
       <c r="Q60" s="0"/>
       <c r="R60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="S60" s="0"/>
       <c r="T60" s="3"/>
       <c r="U60" s="0"/>
       <c r="V60" s="0"/>
       <c r="W60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="X60" s="0"/>
       <c r="Y60" s="3"/>
       <c r="Z60" s="0"/>
       <c r="AA60" s="0"/>
       <c r="AB60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="AC60" s="0"/>
       <c r="AE60" s="0"/>
       <c r="AF60" s="0"/>
       <c r="AG60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="AH60" s="0"/>
       <c r="AJ60" s="0"/>
       <c r="AK60" s="0"/>
       <c r="AL60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="AM60" s="0"/>
       <c r="AN60" s="3"/>
       <c r="AO60" s="0"/>
       <c r="AP60" s="0"/>
       <c r="AQ60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="AR60" s="0"/>
       <c r="AS60" s="0"/>
       <c r="AT60" s="0"/>
       <c r="AU60" s="0"/>
       <c r="AV60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="AW60" s="0"/>
       <c r="AY60" s="0"/>
       <c r="AZ60" s="0"/>
       <c r="BA60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BB60" s="0"/>
       <c r="BC60" s="0"/>
       <c r="BD60" s="0"/>
       <c r="BE60" s="0"/>
       <c r="BF60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BG60" s="0"/>
       <c r="BH60" s="0"/>
       <c r="BI60" s="0"/>
       <c r="BJ60" s="0"/>
       <c r="BK60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BL60" s="0"/>
       <c r="BM60" s="0"/>
       <c r="BN60" s="0"/>
       <c r="BO60" s="0"/>
       <c r="BP60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BQ60" s="0"/>
       <c r="BR60" s="0"/>
       <c r="BS60" s="0"/>
       <c r="BT60" s="0"/>
       <c r="BU60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="BV60" s="0"/>
       <c r="BW60" s="0"/>
       <c r="BX60" s="0"/>
       <c r="BY60" s="0"/>
       <c r="BZ60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CA60" s="0"/>
       <c r="CB60" s="0"/>
       <c r="CC60" s="0"/>
       <c r="CD60" s="0"/>
       <c r="CE60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CF60" s="0"/>
       <c r="CG60" s="0"/>
       <c r="CH60" s="2"/>
       <c r="CI60" s="0"/>
       <c r="CJ60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CK60" s="0"/>
       <c r="CL60" s="0"/>
       <c r="CM60" s="2"/>
       <c r="CN60" s="0"/>
       <c r="CO60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CP60" s="0"/>
       <c r="CQ60" s="0"/>
       <c r="CR60" s="2"/>
       <c r="CS60" s="0"/>
       <c r="CT60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CU60" s="0"/>
       <c r="CV60" s="0"/>
       <c r="CW60" s="2"/>
       <c r="CX60" s="0"/>
       <c r="CY60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="CZ60" s="0"/>
       <c r="DA60" s="0"/>
       <c r="DB60" s="2"/>
       <c r="DC60" s="0"/>
       <c r="DD60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="DE60" s="0"/>
       <c r="DF60" s="0"/>
       <c r="DG60" s="2"/>
       <c r="DH60" s="0"/>
       <c r="DI60" s="78" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="DJ60" s="0"/>
       <c r="DK60" s="0"/>
@@ -65359,158 +65362,158 @@
       <c r="A61" s="0"/>
       <c r="B61" s="0"/>
       <c r="C61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="D61" s="0"/>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
       <c r="G61" s="0"/>
       <c r="H61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="I61" s="0"/>
       <c r="J61" s="0"/>
       <c r="K61" s="0"/>
       <c r="L61" s="0"/>
       <c r="M61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="N61" s="0"/>
       <c r="O61" s="0"/>
       <c r="P61" s="0"/>
       <c r="Q61" s="0"/>
       <c r="R61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="S61" s="0"/>
       <c r="T61" s="3"/>
       <c r="U61" s="0"/>
       <c r="V61" s="0"/>
       <c r="W61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="X61" s="0"/>
       <c r="Y61" s="3"/>
       <c r="Z61" s="0"/>
       <c r="AA61" s="0"/>
       <c r="AB61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="AC61" s="0"/>
       <c r="AE61" s="0"/>
       <c r="AF61" s="0"/>
       <c r="AG61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="AH61" s="0"/>
       <c r="AJ61" s="0"/>
       <c r="AK61" s="0"/>
       <c r="AL61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="AM61" s="0"/>
       <c r="AN61" s="3"/>
       <c r="AO61" s="0"/>
       <c r="AP61" s="0"/>
       <c r="AQ61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="AR61" s="0"/>
       <c r="AS61" s="0"/>
       <c r="AT61" s="0"/>
       <c r="AU61" s="0"/>
       <c r="AV61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="AW61" s="0"/>
       <c r="AY61" s="0"/>
       <c r="AZ61" s="0"/>
       <c r="BA61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="BB61" s="0"/>
       <c r="BC61" s="0"/>
       <c r="BD61" s="0"/>
       <c r="BE61" s="0"/>
       <c r="BF61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="BG61" s="0"/>
       <c r="BH61" s="0"/>
       <c r="BI61" s="0"/>
       <c r="BJ61" s="0"/>
       <c r="BK61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="BL61" s="0"/>
       <c r="BM61" s="0"/>
       <c r="BN61" s="0"/>
       <c r="BO61" s="0"/>
       <c r="BP61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="BQ61" s="0"/>
       <c r="BR61" s="0"/>
       <c r="BS61" s="0"/>
       <c r="BT61" s="0"/>
       <c r="BU61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="BV61" s="0"/>
       <c r="BW61" s="0"/>
       <c r="BX61" s="0"/>
       <c r="BY61" s="0"/>
       <c r="BZ61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CA61" s="0"/>
       <c r="CB61" s="0"/>
       <c r="CC61" s="0"/>
       <c r="CD61" s="0"/>
       <c r="CE61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CF61" s="0"/>
       <c r="CG61" s="0"/>
       <c r="CH61" s="2"/>
       <c r="CI61" s="0"/>
       <c r="CJ61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CK61" s="0"/>
       <c r="CL61" s="0"/>
       <c r="CM61" s="2"/>
       <c r="CN61" s="0"/>
       <c r="CO61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CP61" s="0"/>
       <c r="CQ61" s="0"/>
       <c r="CR61" s="2"/>
       <c r="CS61" s="0"/>
       <c r="CT61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CU61" s="0"/>
       <c r="CV61" s="0"/>
       <c r="CW61" s="2"/>
       <c r="CX61" s="0"/>
       <c r="CY61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="CZ61" s="0"/>
       <c r="DA61" s="0"/>
       <c r="DB61" s="2"/>
       <c r="DC61" s="0"/>
       <c r="DD61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="DE61" s="0"/>
       <c r="DF61" s="0"/>
       <c r="DG61" s="2"/>
       <c r="DH61" s="0"/>
       <c r="DI61" s="79" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="DJ61" s="0"/>
       <c r="DK61" s="0"/>
@@ -65519,158 +65522,158 @@
       <c r="A62" s="0"/>
       <c r="B62" s="0"/>
       <c r="C62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="D62" s="0"/>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
       <c r="G62" s="0"/>
       <c r="H62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="I62" s="0"/>
       <c r="J62" s="0"/>
       <c r="K62" s="0"/>
       <c r="L62" s="0"/>
       <c r="M62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="N62" s="0"/>
       <c r="O62" s="0"/>
       <c r="P62" s="0"/>
       <c r="Q62" s="0"/>
       <c r="R62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="S62" s="0"/>
       <c r="T62" s="3"/>
       <c r="U62" s="0"/>
       <c r="V62" s="0"/>
       <c r="W62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="X62" s="0"/>
       <c r="Y62" s="3"/>
       <c r="Z62" s="0"/>
       <c r="AA62" s="0"/>
       <c r="AB62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="AC62" s="0"/>
       <c r="AE62" s="0"/>
       <c r="AF62" s="0"/>
       <c r="AG62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="AH62" s="0"/>
       <c r="AJ62" s="0"/>
       <c r="AK62" s="0"/>
       <c r="AL62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="AM62" s="0"/>
       <c r="AN62" s="3"/>
       <c r="AO62" s="0"/>
       <c r="AP62" s="0"/>
       <c r="AQ62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="AR62" s="0"/>
       <c r="AS62" s="0"/>
       <c r="AT62" s="0"/>
       <c r="AU62" s="0"/>
       <c r="AV62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="AW62" s="0"/>
       <c r="AY62" s="0"/>
       <c r="AZ62" s="0"/>
       <c r="BA62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="BB62" s="0"/>
       <c r="BC62" s="0"/>
       <c r="BD62" s="0"/>
       <c r="BE62" s="0"/>
       <c r="BF62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="BG62" s="0"/>
       <c r="BH62" s="0"/>
       <c r="BI62" s="0"/>
       <c r="BJ62" s="0"/>
       <c r="BK62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="BL62" s="0"/>
       <c r="BM62" s="0"/>
       <c r="BN62" s="0"/>
       <c r="BO62" s="0"/>
       <c r="BP62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="BQ62" s="0"/>
       <c r="BR62" s="0"/>
       <c r="BS62" s="0"/>
       <c r="BT62" s="0"/>
       <c r="BU62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="BV62" s="0"/>
       <c r="BW62" s="0"/>
       <c r="BX62" s="0"/>
       <c r="BY62" s="0"/>
       <c r="BZ62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CA62" s="0"/>
       <c r="CB62" s="0"/>
       <c r="CC62" s="0"/>
       <c r="CD62" s="0"/>
       <c r="CE62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CF62" s="0"/>
       <c r="CG62" s="0"/>
       <c r="CH62" s="2"/>
       <c r="CI62" s="0"/>
       <c r="CJ62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CK62" s="0"/>
       <c r="CL62" s="0"/>
       <c r="CM62" s="2"/>
       <c r="CN62" s="0"/>
       <c r="CO62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CP62" s="0"/>
       <c r="CQ62" s="0"/>
       <c r="CR62" s="2"/>
       <c r="CS62" s="0"/>
       <c r="CT62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CU62" s="0"/>
       <c r="CV62" s="0"/>
       <c r="CW62" s="2"/>
       <c r="CX62" s="0"/>
       <c r="CY62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="CZ62" s="0"/>
       <c r="DA62" s="0"/>
       <c r="DB62" s="2"/>
       <c r="DC62" s="0"/>
       <c r="DD62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="DE62" s="0"/>
       <c r="DF62" s="0"/>
       <c r="DG62" s="2"/>
       <c r="DH62" s="0"/>
       <c r="DI62" s="37" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="DJ62" s="0"/>
       <c r="DK62" s="0"/>
@@ -65679,316 +65682,316 @@
       <c r="A63" s="0"/>
       <c r="B63" s="0"/>
       <c r="C63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="D63" s="0"/>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
       <c r="G63" s="0"/>
       <c r="H63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="I63" s="0"/>
       <c r="J63" s="0"/>
       <c r="K63" s="0"/>
       <c r="L63" s="0"/>
       <c r="M63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="N63" s="0"/>
       <c r="O63" s="0"/>
       <c r="P63" s="0"/>
       <c r="Q63" s="0"/>
       <c r="R63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="S63" s="0"/>
       <c r="T63" s="3"/>
       <c r="U63" s="0"/>
       <c r="V63" s="0"/>
       <c r="W63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="X63" s="0"/>
       <c r="Y63" s="3"/>
       <c r="Z63" s="0"/>
       <c r="AA63" s="0"/>
       <c r="AB63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="AC63" s="0"/>
       <c r="AE63" s="0"/>
       <c r="AF63" s="0"/>
       <c r="AG63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="AH63" s="0"/>
       <c r="AJ63" s="0"/>
       <c r="AK63" s="0"/>
       <c r="AL63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="AM63" s="0"/>
       <c r="AN63" s="3"/>
       <c r="AO63" s="0"/>
       <c r="AP63" s="0"/>
       <c r="AQ63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="AR63" s="0"/>
       <c r="AS63" s="0"/>
       <c r="AT63" s="0"/>
       <c r="AU63" s="0"/>
       <c r="AV63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="AW63" s="0"/>
       <c r="AY63" s="0"/>
       <c r="AZ63" s="0"/>
       <c r="BA63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="BB63" s="0"/>
       <c r="BC63" s="0"/>
       <c r="BD63" s="0"/>
       <c r="BE63" s="0"/>
       <c r="BF63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="BG63" s="0"/>
       <c r="BH63" s="0"/>
       <c r="BI63" s="0"/>
       <c r="BJ63" s="0"/>
       <c r="BK63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="BL63" s="0"/>
       <c r="BM63" s="0"/>
       <c r="BN63" s="0"/>
       <c r="BO63" s="0"/>
       <c r="BP63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="BQ63" s="0"/>
       <c r="BR63" s="0"/>
       <c r="BS63" s="0"/>
       <c r="BT63" s="0"/>
       <c r="BU63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="BV63" s="0"/>
       <c r="BW63" s="0"/>
       <c r="BX63" s="0"/>
       <c r="BY63" s="0"/>
       <c r="BZ63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CA63" s="0"/>
       <c r="CB63" s="0"/>
       <c r="CC63" s="0"/>
       <c r="CD63" s="0"/>
       <c r="CE63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CF63" s="0"/>
       <c r="CG63" s="0"/>
       <c r="CH63" s="2"/>
       <c r="CI63" s="0"/>
       <c r="CJ63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CK63" s="0"/>
       <c r="CL63" s="0"/>
       <c r="CM63" s="2"/>
       <c r="CN63" s="0"/>
       <c r="CO63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CP63" s="0"/>
       <c r="CQ63" s="0"/>
       <c r="CR63" s="2"/>
       <c r="CS63" s="0"/>
       <c r="CT63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CU63" s="0"/>
       <c r="CV63" s="0"/>
       <c r="CW63" s="2"/>
       <c r="CX63" s="0"/>
       <c r="CY63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="CZ63" s="0"/>
       <c r="DA63" s="0"/>
       <c r="DB63" s="2"/>
       <c r="DC63" s="0"/>
       <c r="DD63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="DE63" s="0"/>
       <c r="DF63" s="0"/>
       <c r="DG63" s="2"/>
       <c r="DH63" s="0"/>
       <c r="DI63" s="36" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="DJ63" s="0"/>
       <c r="DK63" s="0"/>
     </row>
     <row r="64" s="1" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="D64" s="0"/>
       <c r="E64" s="0"/>
       <c r="F64" s="0"/>
       <c r="G64" s="0"/>
       <c r="H64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="I64" s="0"/>
       <c r="J64" s="0"/>
       <c r="K64" s="0"/>
       <c r="L64" s="0"/>
       <c r="M64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="N64" s="0"/>
       <c r="O64" s="0"/>
       <c r="P64" s="0"/>
       <c r="Q64" s="0"/>
       <c r="R64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="S64" s="0"/>
       <c r="T64" s="3"/>
       <c r="U64" s="0"/>
       <c r="V64" s="0"/>
       <c r="W64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="X64" s="0"/>
       <c r="Y64" s="3"/>
       <c r="Z64" s="0"/>
       <c r="AA64" s="0"/>
       <c r="AB64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AC64" s="0"/>
       <c r="AE64" s="0"/>
       <c r="AF64" s="0"/>
       <c r="AG64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AH64" s="0"/>
       <c r="AJ64" s="0"/>
       <c r="AK64" s="0"/>
       <c r="AL64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AM64" s="0"/>
       <c r="AN64" s="3"/>
       <c r="AO64" s="0"/>
       <c r="AP64" s="0"/>
       <c r="AQ64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AR64" s="0"/>
       <c r="AS64" s="0"/>
       <c r="AT64" s="0"/>
       <c r="AU64" s="0"/>
       <c r="AV64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="AW64" s="0"/>
       <c r="AY64" s="0"/>
       <c r="AZ64" s="0"/>
       <c r="BA64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="BB64" s="0"/>
       <c r="BC64" s="0"/>
       <c r="BD64" s="0"/>
       <c r="BE64" s="0"/>
       <c r="BF64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="BG64" s="0"/>
       <c r="BH64" s="0"/>
       <c r="BI64" s="0"/>
       <c r="BJ64" s="0"/>
       <c r="BK64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="BL64" s="0"/>
       <c r="BM64" s="0"/>
       <c r="BN64" s="0"/>
       <c r="BO64" s="0"/>
       <c r="BP64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="BQ64" s="0"/>
       <c r="BR64" s="0"/>
       <c r="BS64" s="0"/>
       <c r="BT64" s="0"/>
       <c r="BU64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="BV64" s="0"/>
       <c r="BW64" s="0"/>
       <c r="BX64" s="0"/>
       <c r="BY64" s="0"/>
       <c r="BZ64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CA64" s="0"/>
       <c r="CB64" s="0"/>
       <c r="CC64" s="0"/>
       <c r="CD64" s="0"/>
       <c r="CE64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CF64" s="0"/>
       <c r="CG64" s="0"/>
       <c r="CH64" s="2"/>
       <c r="CI64" s="0"/>
       <c r="CJ64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CK64" s="0"/>
       <c r="CL64" s="0"/>
       <c r="CM64" s="2"/>
       <c r="CN64" s="0"/>
       <c r="CO64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CP64" s="0"/>
       <c r="CQ64" s="0"/>
       <c r="CR64" s="2"/>
       <c r="CS64" s="0"/>
       <c r="CT64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CU64" s="0"/>
       <c r="CV64" s="0"/>
       <c r="CW64" s="2"/>
       <c r="CX64" s="0"/>
       <c r="CY64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="CZ64" s="0"/>
       <c r="DA64" s="0"/>
       <c r="DB64" s="2"/>
       <c r="DC64" s="0"/>
       <c r="DD64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="DE64" s="0"/>
       <c r="DF64" s="0"/>
       <c r="DG64" s="2"/>
       <c r="DH64" s="0"/>
       <c r="DI64" s="47" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="DJ64" s="0"/>
       <c r="DK64" s="0"/>

</xml_diff>

<commit_message>
add GAYT service for dummy switch service
</commit_message>
<xml_diff>
--- a/flask-backend/Rack Info-201703.xlsx
+++ b/flask-backend/Rack Info-201703.xlsx
@@ -11,13 +11,14 @@
     <sheet name="201703" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_24821951_458D_4863_863B_0C0B4A6350AE_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_F725D54E_BA8A_4561_B030_7A250C390FCD_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_F930B092_4476_4D77_A695_E370DC8CEE30_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'201703'!$A$1:$DK$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_24821951_458D_4863_863B_0C0B4A6350AE_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_F725D54E_BA8A_4561_B030_7A250C390FCD_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_F930B092_4476_4D77_A695_E370DC8CEE30_.wvu.PrintArea" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'201703'!$A$1:$DK$65</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1874" uniqueCount="1061">
   <si>
     <t xml:space="preserve">R00 - R11003</t>
   </si>
@@ -3431,6 +3432,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gcloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GAYT</t>
   </si>
 </sst>
 </file>
@@ -4078,127 +4082,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:63"/>
+  <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A34" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A37" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="3" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="3" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="39" min="39" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="40" min="40" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="41" min="41" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="42" min="42" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="44" min="44" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="45" min="45" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="46" min="46" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="47" min="47" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="49" min="49" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="50" min="50" style="3" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="51" min="51" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="52" min="52" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="54" min="54" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="55" min="55" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="56" min="56" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="57" min="57" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="58" min="58" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="58" min="58" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="59" min="59" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="60" min="60" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="61" min="61" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="62" min="62" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="63" min="63" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="63" min="63" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="64" min="64" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="65" min="65" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="66" min="66" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="67" min="67" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="68" min="68" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="68" min="68" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="69" min="69" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="70" min="70" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="71" min="71" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="72" min="72" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="73" min="73" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="73" min="73" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="74" min="74" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="75" min="75" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="76" min="76" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="77" min="77" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="78" min="78" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="78" min="78" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="79" min="79" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="80" min="80" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="81" min="81" style="2" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="82" min="82" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="83" min="83" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="83" min="83" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="84" min="84" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="85" min="85" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="86" min="86" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="87" min="87" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="88" min="88" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="88" min="88" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="89" min="89" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="90" min="90" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="91" min="91" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="92" min="92" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="93" min="93" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="93" min="93" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="94" min="94" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="95" min="95" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="96" min="96" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="97" min="97" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="98" min="98" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="98" min="98" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="99" min="99" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="100" min="100" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="101" min="101" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="102" min="102" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="103" min="103" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="103" min="103" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="104" min="104" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="105" min="105" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="106" min="106" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="107" min="107" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="108" min="108" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="108" min="108" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="109" min="109" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="110" min="110" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="111" min="111" style="1" width="3.42914979757085"/>
     <col collapsed="false" hidden="false" max="112" min="112" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="113" min="113" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="113" min="113" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="114" min="114" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="115" min="115" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="1025" min="116" style="1" width="9"/>
@@ -63383,6 +63387,123 @@
       <c r="DJ63" s="0"/>
       <c r="DK63" s="0"/>
     </row>
+    <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C64" s="20" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
+      <c r="G64" s="0"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="0"/>
+      <c r="J64" s="0"/>
+      <c r="K64" s="0"/>
+      <c r="L64" s="0"/>
+      <c r="M64" s="36"/>
+      <c r="N64" s="0"/>
+      <c r="O64" s="0"/>
+      <c r="P64" s="0"/>
+      <c r="Q64" s="0"/>
+      <c r="R64" s="36"/>
+      <c r="S64" s="0"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="0"/>
+      <c r="V64" s="0"/>
+      <c r="W64" s="36"/>
+      <c r="X64" s="0"/>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="0"/>
+      <c r="AA64" s="0"/>
+      <c r="AB64" s="36"/>
+      <c r="AC64" s="0"/>
+      <c r="AE64" s="0"/>
+      <c r="AF64" s="0"/>
+      <c r="AG64" s="36"/>
+      <c r="AH64" s="0"/>
+      <c r="AJ64" s="0"/>
+      <c r="AK64" s="0"/>
+      <c r="AL64" s="36"/>
+      <c r="AM64" s="0"/>
+      <c r="AN64" s="3"/>
+      <c r="AO64" s="0"/>
+      <c r="AP64" s="0"/>
+      <c r="AQ64" s="36"/>
+      <c r="AR64" s="0"/>
+      <c r="AS64" s="0"/>
+      <c r="AT64" s="0"/>
+      <c r="AU64" s="0"/>
+      <c r="AV64" s="36"/>
+      <c r="AW64" s="0"/>
+      <c r="AY64" s="0"/>
+      <c r="AZ64" s="0"/>
+      <c r="BA64" s="36"/>
+      <c r="BB64" s="0"/>
+      <c r="BC64" s="0"/>
+      <c r="BD64" s="0"/>
+      <c r="BE64" s="0"/>
+      <c r="BF64" s="36"/>
+      <c r="BG64" s="0"/>
+      <c r="BH64" s="0"/>
+      <c r="BI64" s="0"/>
+      <c r="BJ64" s="0"/>
+      <c r="BK64" s="36"/>
+      <c r="BL64" s="0"/>
+      <c r="BM64" s="0"/>
+      <c r="BN64" s="0"/>
+      <c r="BO64" s="0"/>
+      <c r="BP64" s="36"/>
+      <c r="BQ64" s="0"/>
+      <c r="BR64" s="0"/>
+      <c r="BS64" s="0"/>
+      <c r="BT64" s="0"/>
+      <c r="BU64" s="36"/>
+      <c r="BV64" s="0"/>
+      <c r="BW64" s="0"/>
+      <c r="BX64" s="0"/>
+      <c r="BY64" s="0"/>
+      <c r="BZ64" s="36"/>
+      <c r="CA64" s="0"/>
+      <c r="CB64" s="0"/>
+      <c r="CC64" s="0"/>
+      <c r="CD64" s="0"/>
+      <c r="CE64" s="36"/>
+      <c r="CF64" s="0"/>
+      <c r="CG64" s="0"/>
+      <c r="CH64" s="2"/>
+      <c r="CI64" s="0"/>
+      <c r="CJ64" s="36"/>
+      <c r="CK64" s="0"/>
+      <c r="CL64" s="0"/>
+      <c r="CM64" s="2"/>
+      <c r="CN64" s="0"/>
+      <c r="CO64" s="36"/>
+      <c r="CP64" s="0"/>
+      <c r="CQ64" s="0"/>
+      <c r="CR64" s="2"/>
+      <c r="CS64" s="0"/>
+      <c r="CT64" s="36"/>
+      <c r="CU64" s="0"/>
+      <c r="CV64" s="0"/>
+      <c r="CW64" s="2"/>
+      <c r="CX64" s="0"/>
+      <c r="CY64" s="36"/>
+      <c r="CZ64" s="0"/>
+      <c r="DA64" s="0"/>
+      <c r="DB64" s="2"/>
+      <c r="DC64" s="0"/>
+      <c r="DD64" s="36"/>
+      <c r="DE64" s="0"/>
+      <c r="DF64" s="0"/>
+      <c r="DG64" s="2"/>
+      <c r="DH64" s="0"/>
+      <c r="DI64" s="36"/>
+      <c r="DJ64" s="0"/>
+      <c r="DK64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="269">
     <mergeCell ref="B5:E6"/>

</xml_diff>